<commit_message>
feat: Competition parsing from Excel to class
</commit_message>
<xml_diff>
--- a/Resources/Template_Competition.xlsx
+++ b/Resources/Template_Competition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igor\Programming\Femida\Femida_v0.3\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igor\_Programming\Femida\Femida_v0.3\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D3855D-A804-437C-BEE9-4F8744B8D36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2356E6E0-4E4D-4FB2-B7EE-CF784DE75FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,8 +25,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Igor @cell_laber</author>
+  </authors>
+  <commentList>
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{A52B7A15-9833-4EA1-B553-174E4FF6AE0A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Любое действительное число от -10 до 10</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Результат проверки</t>
   </si>
@@ -116,12 +141,33 @@
     <t>Шаблон проведенного соревнования
 Для использования в учетной базе FEMIDA</t>
   </si>
+  <si>
+    <t>Главный судья соревнований</t>
+  </si>
+  <si>
+    <t>Рефери</t>
+  </si>
+  <si>
+    <t>Руководитель ковра</t>
+  </si>
+  <si>
+    <t>Главный секретарь</t>
+  </si>
+  <si>
+    <t>Секретарь</t>
+  </si>
+  <si>
+    <t>Неизвестно</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Пример оформления даты</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +236,14 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -539,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -703,6 +757,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1276,11 +1333,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AA111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,46 +1351,50 @@
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="24" max="24" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
       <c r="AA2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
       <c r="L3" s="28" t="s">
         <v>9</v>
       </c>
       <c r="M3" s="2"/>
+      <c r="X3" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
@@ -1348,6 +1409,9 @@
       <c r="M4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="X4" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
@@ -1362,6 +1426,9 @@
       <c r="M5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="X5" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
@@ -1378,6 +1445,9 @@
       <c r="M6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="X6" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
@@ -1396,23 +1466,29 @@
       <c r="M7" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="X7" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="59"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="60"/>
       <c r="I8" s="10"/>
       <c r="L8" s="31" t="s">
         <v>15</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1420,12 +1496,16 @@
       <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="62"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="63"/>
       <c r="I9" s="11"/>
+      <c r="L9" s="2"/>
+      <c r="X9" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
@@ -1436,6 +1516,13 @@
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
+      <c r="L10" s="56">
+        <f ca="1">TODAY()</f>
+        <v>44979</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
@@ -1446,6 +1533,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
@@ -1524,7 +1612,7 @@
       <c r="H16" s="21"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1537,7 +1625,7 @@
       <c r="H17" s="21"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1550,7 +1638,7 @@
       <c r="H18" s="21"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1563,7 +1651,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1575,8 +1663,9 @@
       <c r="G20" s="20"/>
       <c r="H20" s="21"/>
       <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1588,8 +1677,9 @@
       <c r="G21" s="20"/>
       <c r="H21" s="21"/>
       <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1601,8 +1691,9 @@
       <c r="G22" s="20"/>
       <c r="H22" s="21"/>
       <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1614,8 +1705,9 @@
       <c r="G23" s="20"/>
       <c r="H23" s="21"/>
       <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1627,8 +1719,9 @@
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
       <c r="I24" s="10"/>
-    </row>
-    <row r="25" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1640,8 +1733,9 @@
       <c r="G25" s="20"/>
       <c r="H25" s="21"/>
       <c r="I25" s="10"/>
-    </row>
-    <row r="26" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1653,8 +1747,9 @@
       <c r="G26" s="20"/>
       <c r="H26" s="21"/>
       <c r="I26" s="10"/>
-    </row>
-    <row r="27" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1667,7 +1762,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1680,7 +1775,7 @@
       <c r="H28" s="21"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1693,7 +1788,7 @@
       <c r="H29" s="21"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1706,7 +1801,7 @@
       <c r="H30" s="21"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1719,7 +1814,7 @@
       <c r="H31" s="21"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2760,6 +2855,7 @@
       <c r="I111" s="11"/>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="3">
     <mergeCell ref="B1:I3"/>
     <mergeCell ref="D8:H8"/>
@@ -2789,7 +2885,22 @@
       <formula>LEN(TRIM(L7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G111" xr:uid="{61BFA409-FA25-4839-9962-B559577D526B}">
+      <formula1>-10</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:H9" xr:uid="{47CE2E7D-C793-4E7D-BFA5-E2B3C6E682EB}">
+      <formula1>36892</formula1>
+      <formula2>401769</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F111" xr:uid="{D3E0206D-FB82-4FC2-A015-9896895148D4}">
+      <formula1>$X$3:$X$9</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2817,37 +2928,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
       <c r="I1" s="32"/>
       <c r="J1" s="33"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
       <c r="I2" s="32"/>
       <c r="J2" s="33"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
       <c r="I3" s="32"/>
       <c r="J3" s="33"/>
     </row>
@@ -2891,11 +3002,11 @@
       <c r="D7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="69" t="str">
+      <c r="E7" s="70" t="str">
         <f>IF(Заполнение!D9="","",Заполнение!D9)</f>
         <v/>
       </c>
-      <c r="F7" s="69"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="35"/>
       <c r="H7" s="37"/>
     </row>
@@ -2924,10 +3035,10 @@
       <c r="C10" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="72"/>
+      <c r="E10" s="73"/>
       <c r="F10" s="42" t="s">
         <v>7</v>
       </c>
@@ -2946,11 +3057,11 @@
         <f>IF(Заполнение!C13="","",Заполнение!C13)</f>
         <v/>
       </c>
-      <c r="D11" s="73" t="str">
+      <c r="D11" s="74" t="str">
         <f>IF(Заполнение!D13="","",Заполнение!D13)</f>
         <v/>
       </c>
-      <c r="E11" s="74"/>
+      <c r="E11" s="75"/>
       <c r="F11" s="46" t="str">
         <f>IF(Заполнение!E13="","",Заполнение!E13)</f>
         <v/>
@@ -2972,11 +3083,11 @@
         <f>IF(Заполнение!C14="","",Заполнение!C14)</f>
         <v/>
       </c>
-      <c r="D12" s="65" t="str">
+      <c r="D12" s="66" t="str">
         <f>IF(Заполнение!D14="","",Заполнение!D14)</f>
         <v/>
       </c>
-      <c r="E12" s="66"/>
+      <c r="E12" s="67"/>
       <c r="F12" s="46" t="str">
         <f>IF(Заполнение!E14="","",Заполнение!E14)</f>
         <v/>
@@ -2999,11 +3110,11 @@
         <f>IF(Заполнение!C15="","",Заполнение!C15)</f>
         <v/>
       </c>
-      <c r="D13" s="65" t="str">
+      <c r="D13" s="66" t="str">
         <f>IF(Заполнение!D15="","",Заполнение!D15)</f>
         <v/>
       </c>
-      <c r="E13" s="66"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="46" t="str">
         <f>IF(Заполнение!E15="","",Заполнение!E15)</f>
         <v/>
@@ -3026,11 +3137,11 @@
         <f>IF(Заполнение!C16="","",Заполнение!C16)</f>
         <v/>
       </c>
-      <c r="D14" s="65" t="str">
+      <c r="D14" s="66" t="str">
         <f>IF(Заполнение!D16="","",Заполнение!D16)</f>
         <v/>
       </c>
-      <c r="E14" s="66"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="46" t="str">
         <f>IF(Заполнение!E16="","",Заполнение!E16)</f>
         <v/>
@@ -3053,11 +3164,11 @@
         <f>IF(Заполнение!C17="","",Заполнение!C17)</f>
         <v/>
       </c>
-      <c r="D15" s="65" t="str">
+      <c r="D15" s="66" t="str">
         <f>IF(Заполнение!D17="","",Заполнение!D17)</f>
         <v/>
       </c>
-      <c r="E15" s="66"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="46" t="str">
         <f>IF(Заполнение!E17="","",Заполнение!E17)</f>
         <v/>
@@ -3080,11 +3191,11 @@
         <f>IF(Заполнение!C18="","",Заполнение!C18)</f>
         <v/>
       </c>
-      <c r="D16" s="65" t="str">
+      <c r="D16" s="66" t="str">
         <f>IF(Заполнение!D18="","",Заполнение!D18)</f>
         <v/>
       </c>
-      <c r="E16" s="66"/>
+      <c r="E16" s="67"/>
       <c r="F16" s="46" t="str">
         <f>IF(Заполнение!E18="","",Заполнение!E18)</f>
         <v/>
@@ -3107,11 +3218,11 @@
         <f>IF(Заполнение!C19="","",Заполнение!C19)</f>
         <v/>
       </c>
-      <c r="D17" s="65" t="str">
+      <c r="D17" s="66" t="str">
         <f>IF(Заполнение!D19="","",Заполнение!D19)</f>
         <v/>
       </c>
-      <c r="E17" s="66"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="46" t="str">
         <f>IF(Заполнение!E19="","",Заполнение!E19)</f>
         <v/>
@@ -3134,11 +3245,11 @@
         <f>IF(Заполнение!C20="","",Заполнение!C20)</f>
         <v/>
       </c>
-      <c r="D18" s="65" t="str">
+      <c r="D18" s="66" t="str">
         <f>IF(Заполнение!D20="","",Заполнение!D20)</f>
         <v/>
       </c>
-      <c r="E18" s="66"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="46" t="str">
         <f>IF(Заполнение!E20="","",Заполнение!E20)</f>
         <v/>
@@ -3161,11 +3272,11 @@
         <f>IF(Заполнение!C21="","",Заполнение!C21)</f>
         <v/>
       </c>
-      <c r="D19" s="65" t="str">
+      <c r="D19" s="66" t="str">
         <f>IF(Заполнение!D21="","",Заполнение!D21)</f>
         <v/>
       </c>
-      <c r="E19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="46" t="str">
         <f>IF(Заполнение!E21="","",Заполнение!E21)</f>
         <v/>
@@ -3188,11 +3299,11 @@
         <f>IF(Заполнение!C22="","",Заполнение!C22)</f>
         <v/>
       </c>
-      <c r="D20" s="65" t="str">
+      <c r="D20" s="66" t="str">
         <f>IF(Заполнение!D22="","",Заполнение!D22)</f>
         <v/>
       </c>
-      <c r="E20" s="66"/>
+      <c r="E20" s="67"/>
       <c r="F20" s="46" t="str">
         <f>IF(Заполнение!E22="","",Заполнение!E22)</f>
         <v/>
@@ -3215,11 +3326,11 @@
         <f>IF(Заполнение!C23="","",Заполнение!C23)</f>
         <v/>
       </c>
-      <c r="D21" s="65" t="str">
+      <c r="D21" s="66" t="str">
         <f>IF(Заполнение!D23="","",Заполнение!D23)</f>
         <v/>
       </c>
-      <c r="E21" s="66"/>
+      <c r="E21" s="67"/>
       <c r="F21" s="46" t="str">
         <f>IF(Заполнение!E23="","",Заполнение!E23)</f>
         <v/>
@@ -3242,11 +3353,11 @@
         <f>IF(Заполнение!C24="","",Заполнение!C24)</f>
         <v/>
       </c>
-      <c r="D22" s="65" t="str">
+      <c r="D22" s="66" t="str">
         <f>IF(Заполнение!D24="","",Заполнение!D24)</f>
         <v/>
       </c>
-      <c r="E22" s="66"/>
+      <c r="E22" s="67"/>
       <c r="F22" s="46" t="str">
         <f>IF(Заполнение!E24="","",Заполнение!E24)</f>
         <v/>
@@ -3269,11 +3380,11 @@
         <f>IF(Заполнение!C25="","",Заполнение!C25)</f>
         <v/>
       </c>
-      <c r="D23" s="65" t="str">
+      <c r="D23" s="66" t="str">
         <f>IF(Заполнение!D25="","",Заполнение!D25)</f>
         <v/>
       </c>
-      <c r="E23" s="66"/>
+      <c r="E23" s="67"/>
       <c r="F23" s="46" t="str">
         <f>IF(Заполнение!E25="","",Заполнение!E25)</f>
         <v/>
@@ -3296,11 +3407,11 @@
         <f>IF(Заполнение!C26="","",Заполнение!C26)</f>
         <v/>
       </c>
-      <c r="D24" s="65" t="str">
+      <c r="D24" s="66" t="str">
         <f>IF(Заполнение!D26="","",Заполнение!D26)</f>
         <v/>
       </c>
-      <c r="E24" s="66"/>
+      <c r="E24" s="67"/>
       <c r="F24" s="46" t="str">
         <f>IF(Заполнение!E26="","",Заполнение!E26)</f>
         <v/>
@@ -3323,11 +3434,11 @@
         <f>IF(Заполнение!C27="","",Заполнение!C27)</f>
         <v/>
       </c>
-      <c r="D25" s="65" t="str">
+      <c r="D25" s="66" t="str">
         <f>IF(Заполнение!D27="","",Заполнение!D27)</f>
         <v/>
       </c>
-      <c r="E25" s="66"/>
+      <c r="E25" s="67"/>
       <c r="F25" s="46" t="str">
         <f>IF(Заполнение!E27="","",Заполнение!E27)</f>
         <v/>
@@ -3350,11 +3461,11 @@
         <f>IF(Заполнение!C28="","",Заполнение!C28)</f>
         <v/>
       </c>
-      <c r="D26" s="65" t="str">
+      <c r="D26" s="66" t="str">
         <f>IF(Заполнение!D28="","",Заполнение!D28)</f>
         <v/>
       </c>
-      <c r="E26" s="66"/>
+      <c r="E26" s="67"/>
       <c r="F26" s="46" t="str">
         <f>IF(Заполнение!E28="","",Заполнение!E28)</f>
         <v/>
@@ -3377,11 +3488,11 @@
         <f>IF(Заполнение!C29="","",Заполнение!C29)</f>
         <v/>
       </c>
-      <c r="D27" s="65" t="str">
+      <c r="D27" s="66" t="str">
         <f>IF(Заполнение!D29="","",Заполнение!D29)</f>
         <v/>
       </c>
-      <c r="E27" s="66"/>
+      <c r="E27" s="67"/>
       <c r="F27" s="46" t="str">
         <f>IF(Заполнение!E29="","",Заполнение!E29)</f>
         <v/>
@@ -3404,11 +3515,11 @@
         <f>IF(Заполнение!C30="","",Заполнение!C30)</f>
         <v/>
       </c>
-      <c r="D28" s="65" t="str">
+      <c r="D28" s="66" t="str">
         <f>IF(Заполнение!D30="","",Заполнение!D30)</f>
         <v/>
       </c>
-      <c r="E28" s="66"/>
+      <c r="E28" s="67"/>
       <c r="F28" s="46" t="str">
         <f>IF(Заполнение!E30="","",Заполнение!E30)</f>
         <v/>
@@ -3431,11 +3542,11 @@
         <f>IF(Заполнение!C31="","",Заполнение!C31)</f>
         <v/>
       </c>
-      <c r="D29" s="65" t="str">
+      <c r="D29" s="66" t="str">
         <f>IF(Заполнение!D31="","",Заполнение!D31)</f>
         <v/>
       </c>
-      <c r="E29" s="66"/>
+      <c r="E29" s="67"/>
       <c r="F29" s="46" t="str">
         <f>IF(Заполнение!E31="","",Заполнение!E31)</f>
         <v/>
@@ -3458,11 +3569,11 @@
         <f>IF(Заполнение!C32="","",Заполнение!C32)</f>
         <v/>
       </c>
-      <c r="D30" s="65" t="str">
+      <c r="D30" s="66" t="str">
         <f>IF(Заполнение!D32="","",Заполнение!D32)</f>
         <v/>
       </c>
-      <c r="E30" s="66"/>
+      <c r="E30" s="67"/>
       <c r="F30" s="46" t="str">
         <f>IF(Заполнение!E32="","",Заполнение!E32)</f>
         <v/>
@@ -3485,11 +3596,11 @@
         <f>IF(Заполнение!C33="","",Заполнение!C33)</f>
         <v/>
       </c>
-      <c r="D31" s="65" t="str">
+      <c r="D31" s="66" t="str">
         <f>IF(Заполнение!D33="","",Заполнение!D33)</f>
         <v/>
       </c>
-      <c r="E31" s="66"/>
+      <c r="E31" s="67"/>
       <c r="F31" s="46" t="str">
         <f>IF(Заполнение!E33="","",Заполнение!E33)</f>
         <v/>
@@ -3512,11 +3623,11 @@
         <f>IF(Заполнение!C34="","",Заполнение!C34)</f>
         <v/>
       </c>
-      <c r="D32" s="65" t="str">
+      <c r="D32" s="66" t="str">
         <f>IF(Заполнение!D34="","",Заполнение!D34)</f>
         <v/>
       </c>
-      <c r="E32" s="66"/>
+      <c r="E32" s="67"/>
       <c r="F32" s="46" t="str">
         <f>IF(Заполнение!E34="","",Заполнение!E34)</f>
         <v/>
@@ -3539,11 +3650,11 @@
         <f>IF(Заполнение!C35="","",Заполнение!C35)</f>
         <v/>
       </c>
-      <c r="D33" s="65" t="str">
+      <c r="D33" s="66" t="str">
         <f>IF(Заполнение!D35="","",Заполнение!D35)</f>
         <v/>
       </c>
-      <c r="E33" s="66"/>
+      <c r="E33" s="67"/>
       <c r="F33" s="46" t="str">
         <f>IF(Заполнение!E35="","",Заполнение!E35)</f>
         <v/>
@@ -3566,11 +3677,11 @@
         <f>IF(Заполнение!C36="","",Заполнение!C36)</f>
         <v/>
       </c>
-      <c r="D34" s="65" t="str">
+      <c r="D34" s="66" t="str">
         <f>IF(Заполнение!D36="","",Заполнение!D36)</f>
         <v/>
       </c>
-      <c r="E34" s="66"/>
+      <c r="E34" s="67"/>
       <c r="F34" s="46" t="str">
         <f>IF(Заполнение!E36="","",Заполнение!E36)</f>
         <v/>
@@ -3593,11 +3704,11 @@
         <f>IF(Заполнение!C37="","",Заполнение!C37)</f>
         <v/>
       </c>
-      <c r="D35" s="65" t="str">
+      <c r="D35" s="66" t="str">
         <f>IF(Заполнение!D37="","",Заполнение!D37)</f>
         <v/>
       </c>
-      <c r="E35" s="66"/>
+      <c r="E35" s="67"/>
       <c r="F35" s="46" t="str">
         <f>IF(Заполнение!E37="","",Заполнение!E37)</f>
         <v/>
@@ -3620,11 +3731,11 @@
         <f>IF(Заполнение!C38="","",Заполнение!C38)</f>
         <v/>
       </c>
-      <c r="D36" s="65" t="str">
+      <c r="D36" s="66" t="str">
         <f>IF(Заполнение!D38="","",Заполнение!D38)</f>
         <v/>
       </c>
-      <c r="E36" s="66"/>
+      <c r="E36" s="67"/>
       <c r="F36" s="46" t="str">
         <f>IF(Заполнение!E38="","",Заполнение!E38)</f>
         <v/>
@@ -3647,11 +3758,11 @@
         <f>IF(Заполнение!C39="","",Заполнение!C39)</f>
         <v/>
       </c>
-      <c r="D37" s="65" t="str">
+      <c r="D37" s="66" t="str">
         <f>IF(Заполнение!D39="","",Заполнение!D39)</f>
         <v/>
       </c>
-      <c r="E37" s="66"/>
+      <c r="E37" s="67"/>
       <c r="F37" s="46" t="str">
         <f>IF(Заполнение!E39="","",Заполнение!E39)</f>
         <v/>
@@ -3674,11 +3785,11 @@
         <f>IF(Заполнение!C40="","",Заполнение!C40)</f>
         <v/>
       </c>
-      <c r="D38" s="65" t="str">
+      <c r="D38" s="66" t="str">
         <f>IF(Заполнение!D40="","",Заполнение!D40)</f>
         <v/>
       </c>
-      <c r="E38" s="66"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="46" t="str">
         <f>IF(Заполнение!E40="","",Заполнение!E40)</f>
         <v/>
@@ -3701,11 +3812,11 @@
         <f>IF(Заполнение!C41="","",Заполнение!C41)</f>
         <v/>
       </c>
-      <c r="D39" s="65" t="str">
+      <c r="D39" s="66" t="str">
         <f>IF(Заполнение!D41="","",Заполнение!D41)</f>
         <v/>
       </c>
-      <c r="E39" s="66"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="46" t="str">
         <f>IF(Заполнение!E41="","",Заполнение!E41)</f>
         <v/>
@@ -3728,11 +3839,11 @@
         <f>IF(Заполнение!C42="","",Заполнение!C42)</f>
         <v/>
       </c>
-      <c r="D40" s="65" t="str">
+      <c r="D40" s="66" t="str">
         <f>IF(Заполнение!D42="","",Заполнение!D42)</f>
         <v/>
       </c>
-      <c r="E40" s="66"/>
+      <c r="E40" s="67"/>
       <c r="F40" s="46" t="str">
         <f>IF(Заполнение!E42="","",Заполнение!E42)</f>
         <v/>
@@ -3755,11 +3866,11 @@
         <f>IF(Заполнение!C43="","",Заполнение!C43)</f>
         <v/>
       </c>
-      <c r="D41" s="65" t="str">
+      <c r="D41" s="66" t="str">
         <f>IF(Заполнение!D43="","",Заполнение!D43)</f>
         <v/>
       </c>
-      <c r="E41" s="66"/>
+      <c r="E41" s="67"/>
       <c r="F41" s="46" t="str">
         <f>IF(Заполнение!E43="","",Заполнение!E43)</f>
         <v/>
@@ -3782,11 +3893,11 @@
         <f>IF(Заполнение!C44="","",Заполнение!C44)</f>
         <v/>
       </c>
-      <c r="D42" s="65" t="str">
+      <c r="D42" s="66" t="str">
         <f>IF(Заполнение!D44="","",Заполнение!D44)</f>
         <v/>
       </c>
-      <c r="E42" s="66"/>
+      <c r="E42" s="67"/>
       <c r="F42" s="46" t="str">
         <f>IF(Заполнение!E44="","",Заполнение!E44)</f>
         <v/>
@@ -3809,11 +3920,11 @@
         <f>IF(Заполнение!C45="","",Заполнение!C45)</f>
         <v/>
       </c>
-      <c r="D43" s="65" t="str">
+      <c r="D43" s="66" t="str">
         <f>IF(Заполнение!D45="","",Заполнение!D45)</f>
         <v/>
       </c>
-      <c r="E43" s="66"/>
+      <c r="E43" s="67"/>
       <c r="F43" s="46" t="str">
         <f>IF(Заполнение!E45="","",Заполнение!E45)</f>
         <v/>
@@ -3836,11 +3947,11 @@
         <f>IF(Заполнение!C46="","",Заполнение!C46)</f>
         <v/>
       </c>
-      <c r="D44" s="65" t="str">
+      <c r="D44" s="66" t="str">
         <f>IF(Заполнение!D46="","",Заполнение!D46)</f>
         <v/>
       </c>
-      <c r="E44" s="66"/>
+      <c r="E44" s="67"/>
       <c r="F44" s="46" t="str">
         <f>IF(Заполнение!E46="","",Заполнение!E46)</f>
         <v/>
@@ -3863,11 +3974,11 @@
         <f>IF(Заполнение!C47="","",Заполнение!C47)</f>
         <v/>
       </c>
-      <c r="D45" s="65" t="str">
+      <c r="D45" s="66" t="str">
         <f>IF(Заполнение!D47="","",Заполнение!D47)</f>
         <v/>
       </c>
-      <c r="E45" s="66"/>
+      <c r="E45" s="67"/>
       <c r="F45" s="46" t="str">
         <f>IF(Заполнение!E47="","",Заполнение!E47)</f>
         <v/>
@@ -3890,11 +4001,11 @@
         <f>IF(Заполнение!C48="","",Заполнение!C48)</f>
         <v/>
       </c>
-      <c r="D46" s="65" t="str">
+      <c r="D46" s="66" t="str">
         <f>IF(Заполнение!D48="","",Заполнение!D48)</f>
         <v/>
       </c>
-      <c r="E46" s="66"/>
+      <c r="E46" s="67"/>
       <c r="F46" s="46" t="str">
         <f>IF(Заполнение!E48="","",Заполнение!E48)</f>
         <v/>
@@ -3917,11 +4028,11 @@
         <f>IF(Заполнение!C49="","",Заполнение!C49)</f>
         <v/>
       </c>
-      <c r="D47" s="65" t="str">
+      <c r="D47" s="66" t="str">
         <f>IF(Заполнение!D49="","",Заполнение!D49)</f>
         <v/>
       </c>
-      <c r="E47" s="66"/>
+      <c r="E47" s="67"/>
       <c r="F47" s="46" t="str">
         <f>IF(Заполнение!E49="","",Заполнение!E49)</f>
         <v/>
@@ -3944,11 +4055,11 @@
         <f>IF(Заполнение!C50="","",Заполнение!C50)</f>
         <v/>
       </c>
-      <c r="D48" s="65" t="str">
+      <c r="D48" s="66" t="str">
         <f>IF(Заполнение!D50="","",Заполнение!D50)</f>
         <v/>
       </c>
-      <c r="E48" s="66"/>
+      <c r="E48" s="67"/>
       <c r="F48" s="46" t="str">
         <f>IF(Заполнение!E50="","",Заполнение!E50)</f>
         <v/>
@@ -3971,11 +4082,11 @@
         <f>IF(Заполнение!C51="","",Заполнение!C51)</f>
         <v/>
       </c>
-      <c r="D49" s="67" t="str">
+      <c r="D49" s="68" t="str">
         <f>IF(Заполнение!D51="","",Заполнение!D51)</f>
         <v/>
       </c>
-      <c r="E49" s="68"/>
+      <c r="E49" s="69"/>
       <c r="F49" s="50" t="str">
         <f>IF(Заполнение!E51="","",Заполнение!E51)</f>
         <v/>
@@ -3990,305 +4101,305 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
       <c r="H50" s="34"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="63" t="s">
+      <c r="B52" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="63"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
-      <c r="F52" s="63"/>
-      <c r="G52" s="70" t="s">
+      <c r="C52" s="64"/>
+      <c r="D52" s="64"/>
+      <c r="E52" s="64"/>
+      <c r="F52" s="64"/>
+      <c r="G52" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="70"/>
+      <c r="H52" s="71"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="63"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="63"/>
-      <c r="F53" s="63"/>
-      <c r="G53" s="70" t="s">
+      <c r="B53" s="64"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="64"/>
+      <c r="G53" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="H53" s="70"/>
+      <c r="H53" s="71"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="63" t="s">
+      <c r="B54" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="63"/>
-      <c r="D54" s="63"/>
-      <c r="E54" s="63"/>
-      <c r="F54" s="63"/>
-      <c r="G54" s="70" t="s">
+      <c r="C54" s="64"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="64"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="H54" s="70"/>
+      <c r="H54" s="71"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D55" s="63"/>
-      <c r="E55" s="63"/>
+      <c r="D55" s="64"/>
+      <c r="E55" s="64"/>
       <c r="H55" s="34"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D56" s="63"/>
-      <c r="E56" s="63"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="64"/>
       <c r="H56" s="34"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="64"/>
       <c r="H57" s="34"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D58" s="63"/>
-      <c r="E58" s="63"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
       <c r="H58" s="34"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D59" s="63"/>
-      <c r="E59" s="63"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
       <c r="H59" s="34"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D63" s="63"/>
-      <c r="E63" s="63"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
       <c r="H63" s="34"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D64" s="63"/>
-      <c r="E64" s="63"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
       <c r="H64" s="34"/>
     </row>
     <row r="65" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D65" s="63"/>
-      <c r="E65" s="63"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
       <c r="H65" s="34"/>
     </row>
     <row r="66" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D66" s="63"/>
-      <c r="E66" s="63"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
       <c r="H66" s="34"/>
     </row>
     <row r="67" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D67" s="63"/>
-      <c r="E67" s="63"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="64"/>
       <c r="H67" s="34"/>
     </row>
     <row r="68" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D68" s="63"/>
-      <c r="E68" s="63"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
       <c r="H68" s="34"/>
     </row>
     <row r="69" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D69" s="63"/>
-      <c r="E69" s="63"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
       <c r="H69" s="34"/>
     </row>
     <row r="70" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D70" s="63"/>
-      <c r="E70" s="63"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="64"/>
       <c r="H70" s="34"/>
     </row>
     <row r="71" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D71" s="63"/>
-      <c r="E71" s="63"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
       <c r="H71" s="34"/>
     </row>
     <row r="72" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="63"/>
-      <c r="E72" s="63"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
       <c r="H72" s="34"/>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="63"/>
-      <c r="E73" s="63"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
       <c r="H73" s="34"/>
     </row>
     <row r="74" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D74" s="63"/>
-      <c r="E74" s="63"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
       <c r="H74" s="34"/>
     </row>
     <row r="75" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D75" s="63"/>
-      <c r="E75" s="63"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
       <c r="H75" s="34"/>
     </row>
     <row r="76" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D76" s="63"/>
-      <c r="E76" s="63"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
       <c r="H76" s="34"/>
     </row>
     <row r="77" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D77" s="63"/>
-      <c r="E77" s="63"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
       <c r="H77" s="34"/>
     </row>
     <row r="78" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D78" s="63"/>
-      <c r="E78" s="63"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
       <c r="H78" s="34"/>
     </row>
     <row r="79" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D79" s="63"/>
-      <c r="E79" s="63"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="64"/>
       <c r="H79" s="34"/>
     </row>
     <row r="80" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D80" s="63"/>
-      <c r="E80" s="63"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
       <c r="H80" s="34"/>
     </row>
     <row r="81" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
       <c r="H81" s="34"/>
     </row>
     <row r="82" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D82" s="63"/>
-      <c r="E82" s="63"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="64"/>
       <c r="H82" s="34"/>
     </row>
     <row r="83" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D83" s="63"/>
-      <c r="E83" s="63"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="64"/>
       <c r="H83" s="34"/>
     </row>
     <row r="84" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D84" s="63"/>
-      <c r="E84" s="63"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
       <c r="H84" s="34"/>
     </row>
     <row r="85" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D85" s="63"/>
-      <c r="E85" s="63"/>
+      <c r="D85" s="64"/>
+      <c r="E85" s="64"/>
       <c r="H85" s="34"/>
     </row>
     <row r="86" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D86" s="63"/>
-      <c r="E86" s="63"/>
+      <c r="D86" s="64"/>
+      <c r="E86" s="64"/>
       <c r="H86" s="34"/>
     </row>
     <row r="87" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D87" s="63"/>
-      <c r="E87" s="63"/>
+      <c r="D87" s="64"/>
+      <c r="E87" s="64"/>
       <c r="H87" s="34"/>
     </row>
     <row r="88" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D88" s="63"/>
-      <c r="E88" s="63"/>
+      <c r="D88" s="64"/>
+      <c r="E88" s="64"/>
       <c r="H88" s="34"/>
     </row>
     <row r="89" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D89" s="63"/>
-      <c r="E89" s="63"/>
+      <c r="D89" s="64"/>
+      <c r="E89" s="64"/>
       <c r="H89" s="34"/>
     </row>
     <row r="90" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D90" s="63"/>
-      <c r="E90" s="63"/>
+      <c r="D90" s="64"/>
+      <c r="E90" s="64"/>
       <c r="H90" s="34"/>
     </row>
     <row r="91" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D91" s="63"/>
-      <c r="E91" s="63"/>
+      <c r="D91" s="64"/>
+      <c r="E91" s="64"/>
       <c r="H91" s="34"/>
     </row>
     <row r="92" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D92" s="63"/>
-      <c r="E92" s="63"/>
+      <c r="D92" s="64"/>
+      <c r="E92" s="64"/>
       <c r="H92" s="34"/>
     </row>
     <row r="93" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D93" s="63"/>
-      <c r="E93" s="63"/>
+      <c r="D93" s="64"/>
+      <c r="E93" s="64"/>
       <c r="H93" s="34"/>
     </row>
     <row r="94" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D94" s="63"/>
-      <c r="E94" s="63"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="64"/>
       <c r="H94" s="34"/>
     </row>
     <row r="95" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D95" s="63"/>
-      <c r="E95" s="63"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="64"/>
       <c r="H95" s="34"/>
     </row>
     <row r="96" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D96" s="63"/>
-      <c r="E96" s="63"/>
+      <c r="D96" s="64"/>
+      <c r="E96" s="64"/>
       <c r="H96" s="34"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D97" s="63"/>
-      <c r="E97" s="63"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="64"/>
       <c r="H97" s="34"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D98" s="63"/>
-      <c r="E98" s="63"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
       <c r="H98" s="34"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D99" s="63"/>
-      <c r="E99" s="63"/>
+      <c r="D99" s="64"/>
+      <c r="E99" s="64"/>
       <c r="H99" s="34"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D100" s="63"/>
-      <c r="E100" s="63"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="64"/>
       <c r="H100" s="34"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D101" s="63"/>
-      <c r="E101" s="63"/>
+      <c r="D101" s="64"/>
+      <c r="E101" s="64"/>
       <c r="H101" s="34"/>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D102" s="63"/>
-      <c r="E102" s="63"/>
+      <c r="D102" s="64"/>
+      <c r="E102" s="64"/>
       <c r="H102" s="34"/>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D103" s="63"/>
-      <c r="E103" s="63"/>
+      <c r="D103" s="64"/>
+      <c r="E103" s="64"/>
       <c r="H103" s="34"/>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D104" s="63"/>
-      <c r="E104" s="63"/>
+      <c r="D104" s="64"/>
+      <c r="E104" s="64"/>
       <c r="H104" s="34"/>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D105" s="63"/>
-      <c r="E105" s="63"/>
+      <c r="D105" s="64"/>
+      <c r="E105" s="64"/>
       <c r="H105" s="34"/>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D106" s="63"/>
-      <c r="E106" s="63"/>
+      <c r="D106" s="64"/>
+      <c r="E106" s="64"/>
       <c r="H106" s="34"/>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D107" s="63"/>
-      <c r="E107" s="63"/>
+      <c r="D107" s="64"/>
+      <c r="E107" s="64"/>
       <c r="H107" s="34"/>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D108" s="63"/>
-      <c r="E108" s="63"/>
+      <c r="D108" s="64"/>
+      <c r="E108" s="64"/>
       <c r="H108" s="34"/>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D109" s="63"/>
-      <c r="E109" s="63"/>
+      <c r="D109" s="64"/>
+      <c r="E109" s="64"/>
       <c r="H109" s="34"/>
     </row>
     <row r="111" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
refactor: changed Resources files and start feature: AddNewReferee
</commit_message>
<xml_diff>
--- a/Resources/Template_Competition.xlsx
+++ b/Resources/Template_Competition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masha\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF219E8-9125-4B9E-8236-CA2895E66945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562CD3AD-A817-4655-8A63-CEBAA8B9161D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,10 +113,6 @@
     <t>Боковой судья</t>
   </si>
   <si>
-    <t>Данные о судейской бригаде, учавствовавшей в соревновании.
-Для формирования рейтинга в учетной базе FEMIDA</t>
-  </si>
-  <si>
     <t>Документ оформлен:</t>
   </si>
   <si>
@@ -158,6 +154,10 @@
   </si>
   <si>
     <t>Ковер</t>
+  </si>
+  <si>
+    <t>Данные о судейской бригаде, участвовавшей в соревновании.
+Для формирования рейтинга в учетной базе FEMIDA</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -766,42 +766,43 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -849,13 +850,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1818589</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>16854</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>287026</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>67996</xdr:rowOff>
@@ -893,13 +894,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>695061</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>12733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1636388</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>34866</xdr:rowOff>
@@ -1204,7 +1205,7 @@
   <dimension ref="B1:Z111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1223,7 @@
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B1" s="57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="57"/>
       <c r="D1" s="57"/>
@@ -1256,7 +1257,7 @@
       </c>
       <c r="L3" s="2"/>
       <c r="W3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1272,7 +1273,7 @@
         <v>9</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1304,7 +1305,7 @@
         <v>11</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1324,7 +1325,7 @@
         <v>13</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1344,7 +1345,7 @@
         <v>15</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1359,7 +1360,7 @@
       <c r="H9" s="63"/>
       <c r="K9" s="2"/>
       <c r="W9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -1372,10 +1373,10 @@
       <c r="H10" s="1"/>
       <c r="K10" s="45">
         <f ca="1">TODAY()</f>
-        <v>44983</v>
+        <v>44988</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:26" s="50" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1408,7 +1409,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="53" t="s">
         <v>17</v>
@@ -2647,1598 +2648,1598 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A082AF-FD51-46DC-B464-1B11CF47559E}">
-  <dimension ref="B1:J110"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="3.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="10" style="23" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="23" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="23" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="3.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="10" style="23" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="23" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="23" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22"/>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="26"/>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="D5" s="27" t="s">
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="28" t="str">
+      <c r="D5" s="28" t="str">
         <f>IF(Заполнение!D7="","",Заполнение!D7)</f>
         <v/>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="26"/>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
-      <c r="D6" s="27" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="C6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="28" t="str">
+      <c r="D6" s="28" t="str">
         <f>IF(Заполнение!D8="","",Заполнение!D8)</f>
         <v/>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="26"/>
-    </row>
-    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="D7" s="27" t="s">
+      <c r="E6" s="28"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="C7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="71" t="str">
+      <c r="D7" s="65" t="str">
         <f>IF(Заполнение!D9="","",Заполнение!D9)</f>
         <v/>
       </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="26"/>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="70">
+      <c r="E7" s="65"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="64">
         <v>1</v>
       </c>
-      <c r="F8" s="70"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="B10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="C10" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="74"/>
-      <c r="F10" s="31" t="s">
+      <c r="D10" s="71"/>
+      <c r="E10" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="F10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="G10" s="29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="33">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
         <v>1</v>
       </c>
-      <c r="C11" s="34" t="str">
+      <c r="B11" s="34" t="str">
         <f>IF(Заполнение!C13="","",Заполнение!C13)</f>
         <v/>
       </c>
-      <c r="D11" s="75" t="str">
+      <c r="C11" s="72" t="str">
         <f>IF(Заполнение!D13="","",Заполнение!D13)</f>
         <v/>
       </c>
-      <c r="E11" s="76"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="35" t="str">
+        <f>IF(Заполнение!E13="","",Заполнение!E13)</f>
+        <v/>
+      </c>
       <c r="F11" s="35" t="str">
-        <f>IF(Заполнение!E13="","",Заполнение!E13)</f>
-        <v/>
-      </c>
-      <c r="G11" s="35" t="str">
         <f>IF(Заполнение!F13="","",Заполнение!F13)</f>
         <v/>
       </c>
-      <c r="H11" s="33" t="str">
+      <c r="G11" s="33" t="str">
         <f>IF(Заполнение!H13="","",Заполнение!H13)</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="33" t="str">
-        <f t="shared" ref="B12" si="0">IF(C12&amp;D12&amp;F12="","",B11+1)</f>
-        <v/>
-      </c>
-      <c r="C12" s="34" t="str">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="str">
+        <f t="shared" ref="A12" si="0">IF(B12&amp;C12&amp;E12="","",A11+1)</f>
+        <v/>
+      </c>
+      <c r="B12" s="34" t="str">
         <f>IF(Заполнение!C14="","",Заполнение!C14)</f>
         <v/>
       </c>
-      <c r="D12" s="66" t="str">
+      <c r="C12" s="68" t="str">
         <f>IF(Заполнение!D14="","",Заполнение!D14)</f>
         <v/>
       </c>
-      <c r="E12" s="67"/>
-      <c r="F12" s="35" t="str">
+      <c r="D12" s="69"/>
+      <c r="E12" s="35" t="str">
         <f>IF(Заполнение!E14="","",Заполнение!E14)</f>
         <v/>
       </c>
-      <c r="G12" s="36" t="str">
+      <c r="F12" s="36" t="str">
         <f>IF(Заполнение!F14="","",Заполнение!F14)</f>
         <v/>
       </c>
-      <c r="H12" s="33" t="str">
+      <c r="G12" s="33" t="str">
         <f>IF(Заполнение!H14="","",Заполнение!H14)</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="33" t="str">
-        <f>IF(C13&amp;D13&amp;F13="","",B12+1)</f>
-        <v/>
-      </c>
-      <c r="C13" s="34" t="str">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="str">
+        <f>IF(B13&amp;C13&amp;E13="","",A12+1)</f>
+        <v/>
+      </c>
+      <c r="B13" s="34" t="str">
         <f>IF(Заполнение!C15="","",Заполнение!C15)</f>
         <v/>
       </c>
-      <c r="D13" s="66" t="str">
+      <c r="C13" s="68" t="str">
         <f>IF(Заполнение!D15="","",Заполнение!D15)</f>
         <v/>
       </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="35" t="str">
+      <c r="D13" s="69"/>
+      <c r="E13" s="35" t="str">
         <f>IF(Заполнение!E15="","",Заполнение!E15)</f>
         <v/>
       </c>
-      <c r="G13" s="36" t="str">
+      <c r="F13" s="36" t="str">
         <f>IF(Заполнение!F15="","",Заполнение!F15)</f>
         <v/>
       </c>
-      <c r="H13" s="33" t="str">
+      <c r="G13" s="33" t="str">
         <f>IF(Заполнение!H15="","",Заполнение!H15)</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="33" t="str">
-        <f t="shared" ref="B14:B48" si="1">IF(C14&amp;D14&amp;F14="","",B13+1)</f>
-        <v/>
-      </c>
-      <c r="C14" s="34" t="str">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="str">
+        <f t="shared" ref="A14:A48" si="1">IF(B14&amp;C14&amp;E14="","",A13+1)</f>
+        <v/>
+      </c>
+      <c r="B14" s="34" t="str">
         <f>IF(Заполнение!C16="","",Заполнение!C16)</f>
         <v/>
       </c>
-      <c r="D14" s="66" t="str">
+      <c r="C14" s="68" t="str">
         <f>IF(Заполнение!D16="","",Заполнение!D16)</f>
         <v/>
       </c>
-      <c r="E14" s="67"/>
-      <c r="F14" s="35" t="str">
+      <c r="D14" s="69"/>
+      <c r="E14" s="35" t="str">
         <f>IF(Заполнение!E16="","",Заполнение!E16)</f>
         <v/>
       </c>
-      <c r="G14" s="36" t="str">
+      <c r="F14" s="36" t="str">
         <f>IF(Заполнение!F16="","",Заполнение!F16)</f>
         <v/>
       </c>
-      <c r="H14" s="33" t="str">
+      <c r="G14" s="33" t="str">
         <f>IF(Заполнение!H16="","",Заполнение!H16)</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C15" s="34" t="str">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B15" s="34" t="str">
         <f>IF(Заполнение!C17="","",Заполнение!C17)</f>
         <v/>
       </c>
-      <c r="D15" s="66" t="str">
+      <c r="C15" s="68" t="str">
         <f>IF(Заполнение!D17="","",Заполнение!D17)</f>
         <v/>
       </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="35" t="str">
+      <c r="D15" s="69"/>
+      <c r="E15" s="35" t="str">
         <f>IF(Заполнение!E17="","",Заполнение!E17)</f>
         <v/>
       </c>
-      <c r="G15" s="36" t="str">
+      <c r="F15" s="36" t="str">
         <f>IF(Заполнение!F17="","",Заполнение!F17)</f>
         <v/>
       </c>
-      <c r="H15" s="33" t="str">
+      <c r="G15" s="33" t="str">
         <f>IF(Заполнение!H17="","",Заполнение!H17)</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C16" s="34" t="str">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B16" s="34" t="str">
         <f>IF(Заполнение!C18="","",Заполнение!C18)</f>
         <v/>
       </c>
-      <c r="D16" s="66" t="str">
+      <c r="C16" s="68" t="str">
         <f>IF(Заполнение!D18="","",Заполнение!D18)</f>
         <v/>
       </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="35" t="str">
+      <c r="D16" s="69"/>
+      <c r="E16" s="35" t="str">
         <f>IF(Заполнение!E18="","",Заполнение!E18)</f>
         <v/>
       </c>
-      <c r="G16" s="36" t="str">
+      <c r="F16" s="36" t="str">
         <f>IF(Заполнение!F18="","",Заполнение!F18)</f>
         <v/>
       </c>
-      <c r="H16" s="33" t="str">
+      <c r="G16" s="33" t="str">
         <f>IF(Заполнение!H18="","",Заполнение!H18)</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C17" s="34" t="str">
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B17" s="34" t="str">
         <f>IF(Заполнение!C19="","",Заполнение!C19)</f>
         <v/>
       </c>
-      <c r="D17" s="66" t="str">
+      <c r="C17" s="68" t="str">
         <f>IF(Заполнение!D19="","",Заполнение!D19)</f>
         <v/>
       </c>
-      <c r="E17" s="67"/>
-      <c r="F17" s="35" t="str">
+      <c r="D17" s="69"/>
+      <c r="E17" s="35" t="str">
         <f>IF(Заполнение!E19="","",Заполнение!E19)</f>
         <v/>
       </c>
-      <c r="G17" s="36" t="str">
+      <c r="F17" s="36" t="str">
         <f>IF(Заполнение!F19="","",Заполнение!F19)</f>
         <v/>
       </c>
-      <c r="H17" s="33" t="str">
+      <c r="G17" s="33" t="str">
         <f>IF(Заполнение!H19="","",Заполнение!H19)</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C18" s="34" t="str">
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B18" s="34" t="str">
         <f>IF(Заполнение!C20="","",Заполнение!C20)</f>
         <v/>
       </c>
-      <c r="D18" s="66" t="str">
+      <c r="C18" s="68" t="str">
         <f>IF(Заполнение!D20="","",Заполнение!D20)</f>
         <v/>
       </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="35" t="str">
+      <c r="D18" s="69"/>
+      <c r="E18" s="35" t="str">
         <f>IF(Заполнение!E20="","",Заполнение!E20)</f>
         <v/>
       </c>
-      <c r="G18" s="36" t="str">
+      <c r="F18" s="36" t="str">
         <f>IF(Заполнение!F20="","",Заполнение!F20)</f>
         <v/>
       </c>
-      <c r="H18" s="33" t="str">
+      <c r="G18" s="33" t="str">
         <f>IF(Заполнение!H20="","",Заполнение!H20)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C19" s="34" t="str">
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B19" s="34" t="str">
         <f>IF(Заполнение!C21="","",Заполнение!C21)</f>
         <v/>
       </c>
-      <c r="D19" s="66" t="str">
+      <c r="C19" s="68" t="str">
         <f>IF(Заполнение!D21="","",Заполнение!D21)</f>
         <v/>
       </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="35" t="str">
+      <c r="D19" s="69"/>
+      <c r="E19" s="35" t="str">
         <f>IF(Заполнение!E21="","",Заполнение!E21)</f>
         <v/>
       </c>
-      <c r="G19" s="36" t="str">
+      <c r="F19" s="36" t="str">
         <f>IF(Заполнение!F21="","",Заполнение!F21)</f>
         <v/>
       </c>
-      <c r="H19" s="33" t="str">
+      <c r="G19" s="33" t="str">
         <f>IF(Заполнение!H21="","",Заполнение!H21)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C20" s="34" t="str">
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B20" s="34" t="str">
         <f>IF(Заполнение!C22="","",Заполнение!C22)</f>
         <v/>
       </c>
-      <c r="D20" s="66" t="str">
+      <c r="C20" s="68" t="str">
         <f>IF(Заполнение!D22="","",Заполнение!D22)</f>
         <v/>
       </c>
-      <c r="E20" s="67"/>
-      <c r="F20" s="35" t="str">
+      <c r="D20" s="69"/>
+      <c r="E20" s="35" t="str">
         <f>IF(Заполнение!E22="","",Заполнение!E22)</f>
         <v/>
       </c>
-      <c r="G20" s="36" t="str">
+      <c r="F20" s="36" t="str">
         <f>IF(Заполнение!F22="","",Заполнение!F22)</f>
         <v/>
       </c>
-      <c r="H20" s="33" t="str">
+      <c r="G20" s="33" t="str">
         <f>IF(Заполнение!H22="","",Заполнение!H22)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C21" s="34" t="str">
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B21" s="34" t="str">
         <f>IF(Заполнение!C23="","",Заполнение!C23)</f>
         <v/>
       </c>
-      <c r="D21" s="66" t="str">
+      <c r="C21" s="68" t="str">
         <f>IF(Заполнение!D23="","",Заполнение!D23)</f>
         <v/>
       </c>
-      <c r="E21" s="67"/>
-      <c r="F21" s="35" t="str">
+      <c r="D21" s="69"/>
+      <c r="E21" s="35" t="str">
         <f>IF(Заполнение!E23="","",Заполнение!E23)</f>
         <v/>
       </c>
-      <c r="G21" s="36" t="str">
+      <c r="F21" s="36" t="str">
         <f>IF(Заполнение!F23="","",Заполнение!F23)</f>
         <v/>
       </c>
-      <c r="H21" s="33" t="str">
+      <c r="G21" s="33" t="str">
         <f>IF(Заполнение!H23="","",Заполнение!H23)</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C22" s="34" t="str">
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B22" s="34" t="str">
         <f>IF(Заполнение!C24="","",Заполнение!C24)</f>
         <v/>
       </c>
-      <c r="D22" s="66" t="str">
+      <c r="C22" s="68" t="str">
         <f>IF(Заполнение!D24="","",Заполнение!D24)</f>
         <v/>
       </c>
-      <c r="E22" s="67"/>
-      <c r="F22" s="35" t="str">
+      <c r="D22" s="69"/>
+      <c r="E22" s="35" t="str">
         <f>IF(Заполнение!E24="","",Заполнение!E24)</f>
         <v/>
       </c>
-      <c r="G22" s="36" t="str">
+      <c r="F22" s="36" t="str">
         <f>IF(Заполнение!F24="","",Заполнение!F24)</f>
         <v/>
       </c>
-      <c r="H22" s="33" t="str">
+      <c r="G22" s="33" t="str">
         <f>IF(Заполнение!H24="","",Заполнение!H24)</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C23" s="34" t="str">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B23" s="34" t="str">
         <f>IF(Заполнение!C25="","",Заполнение!C25)</f>
         <v/>
       </c>
-      <c r="D23" s="66" t="str">
+      <c r="C23" s="68" t="str">
         <f>IF(Заполнение!D25="","",Заполнение!D25)</f>
         <v/>
       </c>
-      <c r="E23" s="67"/>
-      <c r="F23" s="35" t="str">
+      <c r="D23" s="69"/>
+      <c r="E23" s="35" t="str">
         <f>IF(Заполнение!E25="","",Заполнение!E25)</f>
         <v/>
       </c>
-      <c r="G23" s="36" t="str">
+      <c r="F23" s="36" t="str">
         <f>IF(Заполнение!F25="","",Заполнение!F25)</f>
         <v/>
       </c>
-      <c r="H23" s="33" t="str">
+      <c r="G23" s="33" t="str">
         <f>IF(Заполнение!H25="","",Заполнение!H25)</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C24" s="34" t="str">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B24" s="34" t="str">
         <f>IF(Заполнение!C26="","",Заполнение!C26)</f>
         <v/>
       </c>
-      <c r="D24" s="66" t="str">
+      <c r="C24" s="68" t="str">
         <f>IF(Заполнение!D26="","",Заполнение!D26)</f>
         <v/>
       </c>
-      <c r="E24" s="67"/>
-      <c r="F24" s="35" t="str">
+      <c r="D24" s="69"/>
+      <c r="E24" s="35" t="str">
         <f>IF(Заполнение!E26="","",Заполнение!E26)</f>
         <v/>
       </c>
-      <c r="G24" s="36" t="str">
+      <c r="F24" s="36" t="str">
         <f>IF(Заполнение!F26="","",Заполнение!F26)</f>
         <v/>
       </c>
-      <c r="H24" s="33" t="str">
+      <c r="G24" s="33" t="str">
         <f>IF(Заполнение!H26="","",Заполнение!H26)</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C25" s="34" t="str">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B25" s="34" t="str">
         <f>IF(Заполнение!C27="","",Заполнение!C27)</f>
         <v/>
       </c>
-      <c r="D25" s="66" t="str">
+      <c r="C25" s="68" t="str">
         <f>IF(Заполнение!D27="","",Заполнение!D27)</f>
         <v/>
       </c>
-      <c r="E25" s="67"/>
-      <c r="F25" s="35" t="str">
+      <c r="D25" s="69"/>
+      <c r="E25" s="35" t="str">
         <f>IF(Заполнение!E27="","",Заполнение!E27)</f>
         <v/>
       </c>
-      <c r="G25" s="36" t="str">
+      <c r="F25" s="36" t="str">
         <f>IF(Заполнение!F27="","",Заполнение!F27)</f>
         <v/>
       </c>
-      <c r="H25" s="33" t="str">
+      <c r="G25" s="33" t="str">
         <f>IF(Заполнение!H27="","",Заполнение!H27)</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C26" s="34" t="str">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B26" s="34" t="str">
         <f>IF(Заполнение!C28="","",Заполнение!C28)</f>
         <v/>
       </c>
-      <c r="D26" s="66" t="str">
+      <c r="C26" s="68" t="str">
         <f>IF(Заполнение!D28="","",Заполнение!D28)</f>
         <v/>
       </c>
-      <c r="E26" s="67"/>
-      <c r="F26" s="35" t="str">
+      <c r="D26" s="69"/>
+      <c r="E26" s="35" t="str">
         <f>IF(Заполнение!E28="","",Заполнение!E28)</f>
         <v/>
       </c>
-      <c r="G26" s="36" t="str">
+      <c r="F26" s="36" t="str">
         <f>IF(Заполнение!F28="","",Заполнение!F28)</f>
         <v/>
       </c>
-      <c r="H26" s="33" t="str">
+      <c r="G26" s="33" t="str">
         <f>IF(Заполнение!H28="","",Заполнение!H28)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C27" s="34" t="str">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B27" s="34" t="str">
         <f>IF(Заполнение!C29="","",Заполнение!C29)</f>
         <v/>
       </c>
-      <c r="D27" s="66" t="str">
+      <c r="C27" s="68" t="str">
         <f>IF(Заполнение!D29="","",Заполнение!D29)</f>
         <v/>
       </c>
-      <c r="E27" s="67"/>
-      <c r="F27" s="35" t="str">
+      <c r="D27" s="69"/>
+      <c r="E27" s="35" t="str">
         <f>IF(Заполнение!E29="","",Заполнение!E29)</f>
         <v/>
       </c>
-      <c r="G27" s="36" t="str">
+      <c r="F27" s="36" t="str">
         <f>IF(Заполнение!F29="","",Заполнение!F29)</f>
         <v/>
       </c>
-      <c r="H27" s="33" t="str">
+      <c r="G27" s="33" t="str">
         <f>IF(Заполнение!H29="","",Заполнение!H29)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C28" s="34" t="str">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B28" s="34" t="str">
         <f>IF(Заполнение!C30="","",Заполнение!C30)</f>
         <v/>
       </c>
-      <c r="D28" s="66" t="str">
+      <c r="C28" s="68" t="str">
         <f>IF(Заполнение!D30="","",Заполнение!D30)</f>
         <v/>
       </c>
-      <c r="E28" s="67"/>
-      <c r="F28" s="35" t="str">
+      <c r="D28" s="69"/>
+      <c r="E28" s="35" t="str">
         <f>IF(Заполнение!E30="","",Заполнение!E30)</f>
         <v/>
       </c>
-      <c r="G28" s="36" t="str">
+      <c r="F28" s="36" t="str">
         <f>IF(Заполнение!F30="","",Заполнение!F30)</f>
         <v/>
       </c>
-      <c r="H28" s="33" t="str">
+      <c r="G28" s="33" t="str">
         <f>IF(Заполнение!H30="","",Заполнение!H30)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C29" s="34" t="str">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B29" s="34" t="str">
         <f>IF(Заполнение!C31="","",Заполнение!C31)</f>
         <v/>
       </c>
-      <c r="D29" s="66" t="str">
+      <c r="C29" s="68" t="str">
         <f>IF(Заполнение!D31="","",Заполнение!D31)</f>
         <v/>
       </c>
-      <c r="E29" s="67"/>
-      <c r="F29" s="35" t="str">
+      <c r="D29" s="69"/>
+      <c r="E29" s="35" t="str">
         <f>IF(Заполнение!E31="","",Заполнение!E31)</f>
         <v/>
       </c>
-      <c r="G29" s="36" t="str">
+      <c r="F29" s="36" t="str">
         <f>IF(Заполнение!F31="","",Заполнение!F31)</f>
         <v/>
       </c>
-      <c r="H29" s="33" t="str">
+      <c r="G29" s="33" t="str">
         <f>IF(Заполнение!H31="","",Заполнение!H31)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C30" s="34" t="str">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B30" s="34" t="str">
         <f>IF(Заполнение!C32="","",Заполнение!C32)</f>
         <v/>
       </c>
-      <c r="D30" s="66" t="str">
+      <c r="C30" s="68" t="str">
         <f>IF(Заполнение!D32="","",Заполнение!D32)</f>
         <v/>
       </c>
-      <c r="E30" s="67"/>
-      <c r="F30" s="35" t="str">
+      <c r="D30" s="69"/>
+      <c r="E30" s="35" t="str">
         <f>IF(Заполнение!E32="","",Заполнение!E32)</f>
         <v/>
       </c>
-      <c r="G30" s="36" t="str">
+      <c r="F30" s="36" t="str">
         <f>IF(Заполнение!F32="","",Заполнение!F32)</f>
         <v/>
       </c>
-      <c r="H30" s="33" t="str">
+      <c r="G30" s="33" t="str">
         <f>IF(Заполнение!H32="","",Заполнение!H32)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C31" s="34" t="str">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B31" s="34" t="str">
         <f>IF(Заполнение!C33="","",Заполнение!C33)</f>
         <v/>
       </c>
-      <c r="D31" s="66" t="str">
+      <c r="C31" s="68" t="str">
         <f>IF(Заполнение!D33="","",Заполнение!D33)</f>
         <v/>
       </c>
-      <c r="E31" s="67"/>
-      <c r="F31" s="35" t="str">
+      <c r="D31" s="69"/>
+      <c r="E31" s="35" t="str">
         <f>IF(Заполнение!E33="","",Заполнение!E33)</f>
         <v/>
       </c>
-      <c r="G31" s="36" t="str">
+      <c r="F31" s="36" t="str">
         <f>IF(Заполнение!F33="","",Заполнение!F33)</f>
         <v/>
       </c>
-      <c r="H31" s="33" t="str">
+      <c r="G31" s="33" t="str">
         <f>IF(Заполнение!H33="","",Заполнение!H33)</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C32" s="34" t="str">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B32" s="34" t="str">
         <f>IF(Заполнение!C34="","",Заполнение!C34)</f>
         <v/>
       </c>
-      <c r="D32" s="66" t="str">
+      <c r="C32" s="68" t="str">
         <f>IF(Заполнение!D34="","",Заполнение!D34)</f>
         <v/>
       </c>
-      <c r="E32" s="67"/>
-      <c r="F32" s="35" t="str">
+      <c r="D32" s="69"/>
+      <c r="E32" s="35" t="str">
         <f>IF(Заполнение!E34="","",Заполнение!E34)</f>
         <v/>
       </c>
-      <c r="G32" s="36" t="str">
+      <c r="F32" s="36" t="str">
         <f>IF(Заполнение!F34="","",Заполнение!F34)</f>
         <v/>
       </c>
-      <c r="H32" s="33" t="str">
+      <c r="G32" s="33" t="str">
         <f>IF(Заполнение!H34="","",Заполнение!H34)</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C33" s="34" t="str">
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B33" s="34" t="str">
         <f>IF(Заполнение!C35="","",Заполнение!C35)</f>
         <v/>
       </c>
-      <c r="D33" s="66" t="str">
+      <c r="C33" s="68" t="str">
         <f>IF(Заполнение!D35="","",Заполнение!D35)</f>
         <v/>
       </c>
-      <c r="E33" s="67"/>
-      <c r="F33" s="35" t="str">
+      <c r="D33" s="69"/>
+      <c r="E33" s="35" t="str">
         <f>IF(Заполнение!E35="","",Заполнение!E35)</f>
         <v/>
       </c>
-      <c r="G33" s="36" t="str">
+      <c r="F33" s="36" t="str">
         <f>IF(Заполнение!F35="","",Заполнение!F35)</f>
         <v/>
       </c>
-      <c r="H33" s="33" t="str">
+      <c r="G33" s="33" t="str">
         <f>IF(Заполнение!H35="","",Заполнение!H35)</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C34" s="34" t="str">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B34" s="34" t="str">
         <f>IF(Заполнение!C36="","",Заполнение!C36)</f>
         <v/>
       </c>
-      <c r="D34" s="66" t="str">
+      <c r="C34" s="68" t="str">
         <f>IF(Заполнение!D36="","",Заполнение!D36)</f>
         <v/>
       </c>
-      <c r="E34" s="67"/>
-      <c r="F34" s="35" t="str">
+      <c r="D34" s="69"/>
+      <c r="E34" s="35" t="str">
         <f>IF(Заполнение!E36="","",Заполнение!E36)</f>
         <v/>
       </c>
-      <c r="G34" s="36" t="str">
+      <c r="F34" s="36" t="str">
         <f>IF(Заполнение!F36="","",Заполнение!F36)</f>
         <v/>
       </c>
-      <c r="H34" s="33" t="str">
+      <c r="G34" s="33" t="str">
         <f>IF(Заполнение!H36="","",Заполнение!H36)</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C35" s="34" t="str">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B35" s="34" t="str">
         <f>IF(Заполнение!C37="","",Заполнение!C37)</f>
         <v/>
       </c>
-      <c r="D35" s="66" t="str">
+      <c r="C35" s="68" t="str">
         <f>IF(Заполнение!D37="","",Заполнение!D37)</f>
         <v/>
       </c>
-      <c r="E35" s="67"/>
-      <c r="F35" s="35" t="str">
+      <c r="D35" s="69"/>
+      <c r="E35" s="35" t="str">
         <f>IF(Заполнение!E37="","",Заполнение!E37)</f>
         <v/>
       </c>
-      <c r="G35" s="36" t="str">
+      <c r="F35" s="36" t="str">
         <f>IF(Заполнение!F37="","",Заполнение!F37)</f>
         <v/>
       </c>
-      <c r="H35" s="33" t="str">
+      <c r="G35" s="33" t="str">
         <f>IF(Заполнение!H37="","",Заполнение!H37)</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C36" s="34" t="str">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B36" s="34" t="str">
         <f>IF(Заполнение!C38="","",Заполнение!C38)</f>
         <v/>
       </c>
-      <c r="D36" s="66" t="str">
+      <c r="C36" s="68" t="str">
         <f>IF(Заполнение!D38="","",Заполнение!D38)</f>
         <v/>
       </c>
-      <c r="E36" s="67"/>
-      <c r="F36" s="35" t="str">
+      <c r="D36" s="69"/>
+      <c r="E36" s="35" t="str">
         <f>IF(Заполнение!E38="","",Заполнение!E38)</f>
         <v/>
       </c>
-      <c r="G36" s="36" t="str">
+      <c r="F36" s="36" t="str">
         <f>IF(Заполнение!F38="","",Заполнение!F38)</f>
         <v/>
       </c>
-      <c r="H36" s="33" t="str">
+      <c r="G36" s="33" t="str">
         <f>IF(Заполнение!H38="","",Заполнение!H38)</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C37" s="34" t="str">
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B37" s="34" t="str">
         <f>IF(Заполнение!C39="","",Заполнение!C39)</f>
         <v/>
       </c>
-      <c r="D37" s="66" t="str">
+      <c r="C37" s="68" t="str">
         <f>IF(Заполнение!D39="","",Заполнение!D39)</f>
         <v/>
       </c>
-      <c r="E37" s="67"/>
-      <c r="F37" s="35" t="str">
+      <c r="D37" s="69"/>
+      <c r="E37" s="35" t="str">
         <f>IF(Заполнение!E39="","",Заполнение!E39)</f>
         <v/>
       </c>
-      <c r="G37" s="36" t="str">
+      <c r="F37" s="36" t="str">
         <f>IF(Заполнение!F39="","",Заполнение!F39)</f>
         <v/>
       </c>
-      <c r="H37" s="33" t="str">
+      <c r="G37" s="33" t="str">
         <f>IF(Заполнение!H39="","",Заполнение!H39)</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C38" s="34" t="str">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B38" s="34" t="str">
         <f>IF(Заполнение!C40="","",Заполнение!C40)</f>
         <v/>
       </c>
-      <c r="D38" s="66" t="str">
+      <c r="C38" s="68" t="str">
         <f>IF(Заполнение!D40="","",Заполнение!D40)</f>
         <v/>
       </c>
-      <c r="E38" s="67"/>
-      <c r="F38" s="35" t="str">
+      <c r="D38" s="69"/>
+      <c r="E38" s="35" t="str">
         <f>IF(Заполнение!E40="","",Заполнение!E40)</f>
         <v/>
       </c>
-      <c r="G38" s="36" t="str">
+      <c r="F38" s="36" t="str">
         <f>IF(Заполнение!F40="","",Заполнение!F40)</f>
         <v/>
       </c>
-      <c r="H38" s="33" t="str">
+      <c r="G38" s="33" t="str">
         <f>IF(Заполнение!H40="","",Заполнение!H40)</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C39" s="34" t="str">
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B39" s="34" t="str">
         <f>IF(Заполнение!C41="","",Заполнение!C41)</f>
         <v/>
       </c>
-      <c r="D39" s="66" t="str">
+      <c r="C39" s="68" t="str">
         <f>IF(Заполнение!D41="","",Заполнение!D41)</f>
         <v/>
       </c>
-      <c r="E39" s="67"/>
-      <c r="F39" s="35" t="str">
+      <c r="D39" s="69"/>
+      <c r="E39" s="35" t="str">
         <f>IF(Заполнение!E41="","",Заполнение!E41)</f>
         <v/>
       </c>
-      <c r="G39" s="36" t="str">
+      <c r="F39" s="36" t="str">
         <f>IF(Заполнение!F41="","",Заполнение!F41)</f>
         <v/>
       </c>
-      <c r="H39" s="33" t="str">
+      <c r="G39" s="33" t="str">
         <f>IF(Заполнение!H41="","",Заполнение!H41)</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C40" s="34" t="str">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B40" s="34" t="str">
         <f>IF(Заполнение!C42="","",Заполнение!C42)</f>
         <v/>
       </c>
-      <c r="D40" s="66" t="str">
+      <c r="C40" s="68" t="str">
         <f>IF(Заполнение!D42="","",Заполнение!D42)</f>
         <v/>
       </c>
-      <c r="E40" s="67"/>
-      <c r="F40" s="35" t="str">
+      <c r="D40" s="69"/>
+      <c r="E40" s="35" t="str">
         <f>IF(Заполнение!E42="","",Заполнение!E42)</f>
         <v/>
       </c>
-      <c r="G40" s="36" t="str">
+      <c r="F40" s="36" t="str">
         <f>IF(Заполнение!F42="","",Заполнение!F42)</f>
         <v/>
       </c>
-      <c r="H40" s="33" t="str">
+      <c r="G40" s="33" t="str">
         <f>IF(Заполнение!H42="","",Заполнение!H42)</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C41" s="34" t="str">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B41" s="34" t="str">
         <f>IF(Заполнение!C43="","",Заполнение!C43)</f>
         <v/>
       </c>
-      <c r="D41" s="66" t="str">
+      <c r="C41" s="68" t="str">
         <f>IF(Заполнение!D43="","",Заполнение!D43)</f>
         <v/>
       </c>
-      <c r="E41" s="67"/>
-      <c r="F41" s="35" t="str">
+      <c r="D41" s="69"/>
+      <c r="E41" s="35" t="str">
         <f>IF(Заполнение!E43="","",Заполнение!E43)</f>
         <v/>
       </c>
-      <c r="G41" s="36" t="str">
+      <c r="F41" s="36" t="str">
         <f>IF(Заполнение!F43="","",Заполнение!F43)</f>
         <v/>
       </c>
-      <c r="H41" s="33" t="str">
+      <c r="G41" s="33" t="str">
         <f>IF(Заполнение!H43="","",Заполнение!H43)</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C42" s="34" t="str">
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B42" s="34" t="str">
         <f>IF(Заполнение!C44="","",Заполнение!C44)</f>
         <v/>
       </c>
-      <c r="D42" s="66" t="str">
+      <c r="C42" s="68" t="str">
         <f>IF(Заполнение!D44="","",Заполнение!D44)</f>
         <v/>
       </c>
-      <c r="E42" s="67"/>
-      <c r="F42" s="35" t="str">
+      <c r="D42" s="69"/>
+      <c r="E42" s="35" t="str">
         <f>IF(Заполнение!E44="","",Заполнение!E44)</f>
         <v/>
       </c>
-      <c r="G42" s="36" t="str">
+      <c r="F42" s="36" t="str">
         <f>IF(Заполнение!F44="","",Заполнение!F44)</f>
         <v/>
       </c>
-      <c r="H42" s="33" t="str">
+      <c r="G42" s="33" t="str">
         <f>IF(Заполнение!H44="","",Заполнение!H44)</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C43" s="34" t="str">
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B43" s="34" t="str">
         <f>IF(Заполнение!C45="","",Заполнение!C45)</f>
         <v/>
       </c>
-      <c r="D43" s="66" t="str">
+      <c r="C43" s="68" t="str">
         <f>IF(Заполнение!D45="","",Заполнение!D45)</f>
         <v/>
       </c>
-      <c r="E43" s="67"/>
-      <c r="F43" s="35" t="str">
+      <c r="D43" s="69"/>
+      <c r="E43" s="35" t="str">
         <f>IF(Заполнение!E45="","",Заполнение!E45)</f>
         <v/>
       </c>
-      <c r="G43" s="36" t="str">
+      <c r="F43" s="36" t="str">
         <f>IF(Заполнение!F45="","",Заполнение!F45)</f>
         <v/>
       </c>
-      <c r="H43" s="33" t="str">
+      <c r="G43" s="33" t="str">
         <f>IF(Заполнение!H45="","",Заполнение!H45)</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C44" s="34" t="str">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B44" s="34" t="str">
         <f>IF(Заполнение!C46="","",Заполнение!C46)</f>
         <v/>
       </c>
-      <c r="D44" s="66" t="str">
+      <c r="C44" s="68" t="str">
         <f>IF(Заполнение!D46="","",Заполнение!D46)</f>
         <v/>
       </c>
-      <c r="E44" s="67"/>
-      <c r="F44" s="35" t="str">
+      <c r="D44" s="69"/>
+      <c r="E44" s="35" t="str">
         <f>IF(Заполнение!E46="","",Заполнение!E46)</f>
         <v/>
       </c>
-      <c r="G44" s="36" t="str">
+      <c r="F44" s="36" t="str">
         <f>IF(Заполнение!F46="","",Заполнение!F46)</f>
         <v/>
       </c>
-      <c r="H44" s="33" t="str">
+      <c r="G44" s="33" t="str">
         <f>IF(Заполнение!H46="","",Заполнение!H46)</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C45" s="34" t="str">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B45" s="34" t="str">
         <f>IF(Заполнение!C47="","",Заполнение!C47)</f>
         <v/>
       </c>
-      <c r="D45" s="66" t="str">
+      <c r="C45" s="68" t="str">
         <f>IF(Заполнение!D47="","",Заполнение!D47)</f>
         <v/>
       </c>
-      <c r="E45" s="67"/>
-      <c r="F45" s="35" t="str">
+      <c r="D45" s="69"/>
+      <c r="E45" s="35" t="str">
         <f>IF(Заполнение!E47="","",Заполнение!E47)</f>
         <v/>
       </c>
-      <c r="G45" s="36" t="str">
+      <c r="F45" s="36" t="str">
         <f>IF(Заполнение!F47="","",Заполнение!F47)</f>
         <v/>
       </c>
-      <c r="H45" s="33" t="str">
+      <c r="G45" s="33" t="str">
         <f>IF(Заполнение!H47="","",Заполнение!H47)</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C46" s="34" t="str">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B46" s="34" t="str">
         <f>IF(Заполнение!C48="","",Заполнение!C48)</f>
         <v/>
       </c>
-      <c r="D46" s="66" t="str">
+      <c r="C46" s="68" t="str">
         <f>IF(Заполнение!D48="","",Заполнение!D48)</f>
         <v/>
       </c>
-      <c r="E46" s="67"/>
-      <c r="F46" s="35" t="str">
+      <c r="D46" s="69"/>
+      <c r="E46" s="35" t="str">
         <f>IF(Заполнение!E48="","",Заполнение!E48)</f>
         <v/>
       </c>
-      <c r="G46" s="36" t="str">
+      <c r="F46" s="36" t="str">
         <f>IF(Заполнение!F48="","",Заполнение!F48)</f>
         <v/>
       </c>
-      <c r="H46" s="33" t="str">
+      <c r="G46" s="33" t="str">
         <f>IF(Заполнение!H48="","",Заполнение!H48)</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C47" s="34" t="str">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B47" s="34" t="str">
         <f>IF(Заполнение!C49="","",Заполнение!C49)</f>
         <v/>
       </c>
-      <c r="D47" s="66" t="str">
+      <c r="C47" s="68" t="str">
         <f>IF(Заполнение!D49="","",Заполнение!D49)</f>
         <v/>
       </c>
-      <c r="E47" s="67"/>
-      <c r="F47" s="35" t="str">
+      <c r="D47" s="69"/>
+      <c r="E47" s="35" t="str">
         <f>IF(Заполнение!E49="","",Заполнение!E49)</f>
         <v/>
       </c>
-      <c r="G47" s="36" t="str">
+      <c r="F47" s="36" t="str">
         <f>IF(Заполнение!F49="","",Заполнение!F49)</f>
         <v/>
       </c>
-      <c r="H47" s="33" t="str">
+      <c r="G47" s="33" t="str">
         <f>IF(Заполнение!H49="","",Заполнение!H49)</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="49" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C48" s="38" t="str">
+    <row r="48" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B48" s="38" t="str">
         <f>IF(Заполнение!C50="","",Заполнение!C50)</f>
         <v/>
       </c>
-      <c r="D48" s="68" t="str">
+      <c r="C48" s="75" t="str">
         <f>IF(Заполнение!D50="","",Заполнение!D50)</f>
         <v/>
       </c>
-      <c r="E48" s="69"/>
-      <c r="F48" s="39" t="str">
+      <c r="D48" s="76"/>
+      <c r="E48" s="39" t="str">
         <f>IF(Заполнение!E50="","",Заполнение!E50)</f>
         <v/>
       </c>
-      <c r="G48" s="40" t="str">
+      <c r="F48" s="40" t="str">
         <f>IF(Заполнение!F50="","",Заполнение!F50)</f>
         <v/>
       </c>
-      <c r="H48" s="37" t="str">
+      <c r="G48" s="37" t="str">
         <f>IF(Заполнение!H50="","",Заполнение!H50)</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="H49" s="23"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="72" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
+      <c r="G49" s="23"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="66"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="66"/>
+      <c r="F51" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="67"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="66"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" s="67"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="H51" s="72"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="64"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="H52" s="72"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="72" t="str">
+      <c r="B53" s="66"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="67" t="str">
         <f ca="1">"Дата: " &amp; TEXT(TODAY(),"ДД.ММ.ГГГГ")</f>
-        <v>Дата: 26.02.2023</v>
-      </c>
-      <c r="H53" s="72"/>
-      <c r="J53" s="46"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
-      <c r="H54" s="23"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D55" s="64"/>
-      <c r="E55" s="64"/>
-      <c r="H55" s="23"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
-      <c r="H56" s="23"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D57" s="64"/>
-      <c r="E57" s="64"/>
-      <c r="H57" s="23"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D58" s="64"/>
-      <c r="E58" s="64"/>
-      <c r="H58" s="23"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D62" s="64"/>
-      <c r="E62" s="64"/>
-      <c r="H62" s="23"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="H63" s="23"/>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D64" s="64"/>
-      <c r="E64" s="64"/>
-      <c r="H64" s="23"/>
-    </row>
-    <row r="65" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D65" s="64"/>
-      <c r="E65" s="64"/>
-      <c r="H65" s="23"/>
-    </row>
-    <row r="66" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D66" s="64"/>
-      <c r="E66" s="64"/>
-      <c r="H66" s="23"/>
-    </row>
-    <row r="67" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D67" s="64"/>
-      <c r="E67" s="64"/>
-      <c r="H67" s="23"/>
-    </row>
-    <row r="68" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D68" s="64"/>
-      <c r="E68" s="64"/>
-      <c r="H68" s="23"/>
-    </row>
-    <row r="69" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D69" s="64"/>
-      <c r="E69" s="64"/>
-      <c r="H69" s="23"/>
-    </row>
-    <row r="70" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D70" s="64"/>
-      <c r="E70" s="64"/>
-      <c r="H70" s="23"/>
-    </row>
-    <row r="71" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D71" s="64"/>
-      <c r="E71" s="64"/>
-      <c r="H71" s="23"/>
-    </row>
-    <row r="72" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="64"/>
-      <c r="E72" s="64"/>
-      <c r="H72" s="23"/>
-    </row>
-    <row r="73" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="64"/>
-      <c r="E73" s="64"/>
-      <c r="H73" s="23"/>
-    </row>
-    <row r="74" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D74" s="64"/>
-      <c r="E74" s="64"/>
-      <c r="H74" s="23"/>
-    </row>
-    <row r="75" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D75" s="64"/>
-      <c r="E75" s="64"/>
-      <c r="H75" s="23"/>
-    </row>
-    <row r="76" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D76" s="64"/>
-      <c r="E76" s="64"/>
-      <c r="H76" s="23"/>
-    </row>
-    <row r="77" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D77" s="64"/>
-      <c r="E77" s="64"/>
-      <c r="H77" s="23"/>
-    </row>
-    <row r="78" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D78" s="64"/>
-      <c r="E78" s="64"/>
-      <c r="H78" s="23"/>
-    </row>
-    <row r="79" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D79" s="64"/>
-      <c r="E79" s="64"/>
-      <c r="H79" s="23"/>
-    </row>
-    <row r="80" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D80" s="64"/>
-      <c r="E80" s="64"/>
-      <c r="H80" s="23"/>
-    </row>
-    <row r="81" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D81" s="64"/>
-      <c r="E81" s="64"/>
-      <c r="H81" s="23"/>
-    </row>
-    <row r="82" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D82" s="64"/>
-      <c r="E82" s="64"/>
-      <c r="H82" s="23"/>
-    </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D83" s="64"/>
-      <c r="E83" s="64"/>
-      <c r="H83" s="23"/>
-    </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D84" s="64"/>
-      <c r="E84" s="64"/>
-      <c r="H84" s="23"/>
-    </row>
-    <row r="85" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D85" s="64"/>
-      <c r="E85" s="64"/>
-      <c r="H85" s="23"/>
-    </row>
-    <row r="86" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D86" s="64"/>
-      <c r="E86" s="64"/>
-      <c r="H86" s="23"/>
-    </row>
-    <row r="87" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D87" s="64"/>
-      <c r="E87" s="64"/>
-      <c r="H87" s="23"/>
-    </row>
-    <row r="88" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D88" s="64"/>
-      <c r="E88" s="64"/>
-      <c r="H88" s="23"/>
-    </row>
-    <row r="89" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D89" s="64"/>
-      <c r="E89" s="64"/>
-      <c r="H89" s="23"/>
-    </row>
-    <row r="90" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D90" s="64"/>
-      <c r="E90" s="64"/>
-      <c r="H90" s="23"/>
-    </row>
-    <row r="91" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D91" s="64"/>
-      <c r="E91" s="64"/>
-      <c r="H91" s="23"/>
-    </row>
-    <row r="92" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D92" s="64"/>
-      <c r="E92" s="64"/>
-      <c r="H92" s="23"/>
-    </row>
-    <row r="93" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D93" s="64"/>
-      <c r="E93" s="64"/>
-      <c r="H93" s="23"/>
-    </row>
-    <row r="94" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D94" s="64"/>
-      <c r="E94" s="64"/>
-      <c r="H94" s="23"/>
-    </row>
-    <row r="95" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D95" s="64"/>
-      <c r="E95" s="64"/>
-      <c r="H95" s="23"/>
-    </row>
-    <row r="96" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D96" s="64"/>
-      <c r="E96" s="64"/>
-      <c r="H96" s="23"/>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D97" s="64"/>
-      <c r="E97" s="64"/>
-      <c r="H97" s="23"/>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D98" s="64"/>
-      <c r="E98" s="64"/>
-      <c r="H98" s="23"/>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D99" s="64"/>
-      <c r="E99" s="64"/>
-      <c r="H99" s="23"/>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D100" s="64"/>
-      <c r="E100" s="64"/>
-      <c r="H100" s="23"/>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D101" s="64"/>
-      <c r="E101" s="64"/>
-      <c r="H101" s="23"/>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D102" s="64"/>
-      <c r="E102" s="64"/>
-      <c r="H102" s="23"/>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D103" s="64"/>
-      <c r="E103" s="64"/>
-      <c r="H103" s="23"/>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D104" s="64"/>
-      <c r="E104" s="64"/>
-      <c r="H104" s="23"/>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D105" s="64"/>
-      <c r="E105" s="64"/>
-      <c r="H105" s="23"/>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D106" s="64"/>
-      <c r="E106" s="64"/>
-      <c r="H106" s="23"/>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D107" s="64"/>
-      <c r="E107" s="64"/>
-      <c r="H107" s="23"/>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D108" s="64"/>
-      <c r="E108" s="64"/>
-      <c r="H108" s="23"/>
-    </row>
-    <row r="110" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B110" s="41"/>
+        <v>Дата: 03.03.2023</v>
+      </c>
+      <c r="G53" s="67"/>
+      <c r="I53" s="46"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C54" s="74"/>
+      <c r="D54" s="74"/>
+      <c r="G54" s="23"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C55" s="74"/>
+      <c r="D55" s="74"/>
+      <c r="G55" s="23"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C56" s="74"/>
+      <c r="D56" s="74"/>
+      <c r="G56" s="23"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C57" s="74"/>
+      <c r="D57" s="74"/>
+      <c r="G57" s="23"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
+      <c r="G58" s="23"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C62" s="74"/>
+      <c r="D62" s="74"/>
+      <c r="G62" s="23"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C63" s="74"/>
+      <c r="D63" s="74"/>
+      <c r="G63" s="23"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C64" s="74"/>
+      <c r="D64" s="74"/>
+      <c r="G64" s="23"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65" s="74"/>
+      <c r="D65" s="74"/>
+      <c r="G65" s="23"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C66" s="74"/>
+      <c r="D66" s="74"/>
+      <c r="G66" s="23"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C67" s="74"/>
+      <c r="D67" s="74"/>
+      <c r="G67" s="23"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="74"/>
+      <c r="D68" s="74"/>
+      <c r="G68" s="23"/>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C69" s="74"/>
+      <c r="D69" s="74"/>
+      <c r="G69" s="23"/>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C70" s="74"/>
+      <c r="D70" s="74"/>
+      <c r="G70" s="23"/>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C71" s="74"/>
+      <c r="D71" s="74"/>
+      <c r="G71" s="23"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C72" s="74"/>
+      <c r="D72" s="74"/>
+      <c r="G72" s="23"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C73" s="74"/>
+      <c r="D73" s="74"/>
+      <c r="G73" s="23"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C74" s="74"/>
+      <c r="D74" s="74"/>
+      <c r="G74" s="23"/>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C75" s="74"/>
+      <c r="D75" s="74"/>
+      <c r="G75" s="23"/>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C76" s="74"/>
+      <c r="D76" s="74"/>
+      <c r="G76" s="23"/>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C77" s="74"/>
+      <c r="D77" s="74"/>
+      <c r="G77" s="23"/>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C78" s="74"/>
+      <c r="D78" s="74"/>
+      <c r="G78" s="23"/>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C79" s="74"/>
+      <c r="D79" s="74"/>
+      <c r="G79" s="23"/>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C80" s="74"/>
+      <c r="D80" s="74"/>
+      <c r="G80" s="23"/>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C81" s="74"/>
+      <c r="D81" s="74"/>
+      <c r="G81" s="23"/>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C82" s="74"/>
+      <c r="D82" s="74"/>
+      <c r="G82" s="23"/>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C83" s="74"/>
+      <c r="D83" s="74"/>
+      <c r="G83" s="23"/>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C84" s="74"/>
+      <c r="D84" s="74"/>
+      <c r="G84" s="23"/>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C85" s="74"/>
+      <c r="D85" s="74"/>
+      <c r="G85" s="23"/>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C86" s="74"/>
+      <c r="D86" s="74"/>
+      <c r="G86" s="23"/>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C87" s="74"/>
+      <c r="D87" s="74"/>
+      <c r="G87" s="23"/>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C88" s="74"/>
+      <c r="D88" s="74"/>
+      <c r="G88" s="23"/>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C89" s="74"/>
+      <c r="D89" s="74"/>
+      <c r="G89" s="23"/>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C90" s="74"/>
+      <c r="D90" s="74"/>
+      <c r="G90" s="23"/>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C91" s="74"/>
+      <c r="D91" s="74"/>
+      <c r="G91" s="23"/>
+    </row>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C92" s="74"/>
+      <c r="D92" s="74"/>
+      <c r="G92" s="23"/>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C93" s="74"/>
+      <c r="D93" s="74"/>
+      <c r="G93" s="23"/>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C94" s="74"/>
+      <c r="D94" s="74"/>
+      <c r="G94" s="23"/>
+    </row>
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C95" s="74"/>
+      <c r="D95" s="74"/>
+      <c r="G95" s="23"/>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C96" s="74"/>
+      <c r="D96" s="74"/>
+      <c r="G96" s="23"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C97" s="74"/>
+      <c r="D97" s="74"/>
+      <c r="G97" s="23"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C98" s="74"/>
+      <c r="D98" s="74"/>
+      <c r="G98" s="23"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C99" s="74"/>
+      <c r="D99" s="74"/>
+      <c r="G99" s="23"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C100" s="74"/>
+      <c r="D100" s="74"/>
+      <c r="G100" s="23"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C101" s="74"/>
+      <c r="D101" s="74"/>
+      <c r="G101" s="23"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C102" s="74"/>
+      <c r="D102" s="74"/>
+      <c r="G102" s="23"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C103" s="74"/>
+      <c r="D103" s="74"/>
+      <c r="G103" s="23"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C104" s="74"/>
+      <c r="D104" s="74"/>
+      <c r="G104" s="23"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C105" s="74"/>
+      <c r="D105" s="74"/>
+      <c r="G105" s="23"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C106" s="74"/>
+      <c r="D106" s="74"/>
+      <c r="G106" s="23"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C107" s="74"/>
+      <c r="D107" s="74"/>
+      <c r="G107" s="23"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C108" s="74"/>
+      <c r="D108" s="74"/>
+      <c r="G108" s="23"/>
+    </row>
+    <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="41"/>
+      <c r="B110" s="42"/>
       <c r="C110" s="42"/>
-      <c r="D110" s="42"/>
-      <c r="E110" s="43"/>
+      <c r="D110" s="43"/>
+      <c r="E110" s="42"/>
       <c r="F110" s="42"/>
-      <c r="G110" s="42"/>
-      <c r="H110" s="41"/>
-      <c r="I110" s="42"/>
-      <c r="J110" s="41"/>
+      <c r="G110" s="41"/>
+      <c r="H110" s="42"/>
+      <c r="I110" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="101">
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="B1:H3"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="A1:G3"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <pageMargins left="0.32" right="0.11" top="0.23622047244094491" bottom="0" header="0" footer="0.08"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: adding new referee to the DB. Need a refactor
</commit_message>
<xml_diff>
--- a/Resources/Template_Competition.xlsx
+++ b/Resources/Template_Competition.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562CD3AD-A817-4655-8A63-CEBAA8B9161D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A28D91-933E-4BA9-B642-3C71A293A407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заполнение" sheetId="1" r:id="rId1"/>
     <sheet name="Печать" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -51,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Название соревнования:</t>
   </si>
@@ -158,6 +167,18 @@
   <si>
     <t>Данные о судейской бригаде, участвовавшей в соревновании.
 Для формирования рейтинга в учетной базе FEMIDA</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>dsa</t>
+  </si>
+  <si>
+    <t>sd</t>
   </si>
 </sst>
 </file>
@@ -766,6 +787,22 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -776,12 +813,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -793,16 +824,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1205,7 +1226,7 @@
   <dimension ref="B1:Z111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1334,9 @@
       <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="58"/>
+      <c r="D7" s="58" t="s">
+        <v>35</v>
+      </c>
       <c r="E7" s="59"/>
       <c r="F7" s="59"/>
       <c r="G7" s="59"/>
@@ -1333,7 +1356,9 @@
       <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="58"/>
+      <c r="D8" s="58" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="59"/>
       <c r="F8" s="59"/>
       <c r="G8" s="59"/>
@@ -1353,7 +1378,9 @@
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="61">
+        <v>45004</v>
+      </c>
       <c r="E9" s="62"/>
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
@@ -1373,7 +1400,7 @@
       <c r="H10" s="1"/>
       <c r="K10" s="45">
         <f ca="1">TODAY()</f>
-        <v>44988</v>
+        <v>45004</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>30</v>
@@ -1419,12 +1446,24 @@
       <c r="B13" s="10">
         <v>1</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="47"/>
+      <c r="C13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="47">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="str">
@@ -2669,37 +2708,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
       <c r="H1" s="21"/>
       <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
       <c r="H2" s="21"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
       <c r="H3" s="21"/>
       <c r="I3" s="22"/>
     </row>
@@ -2719,7 +2758,7 @@
       </c>
       <c r="D5" s="28" t="str">
         <f>IF(Заполнение!D7="","",Заполнение!D7)</f>
-        <v/>
+        <v>sdf</v>
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="24"/>
@@ -2732,7 +2771,7 @@
       </c>
       <c r="D6" s="28" t="str">
         <f>IF(Заполнение!D8="","",Заполнение!D8)</f>
-        <v/>
+        <v>sdf</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="24"/>
@@ -2743,11 +2782,11 @@
       <c r="C7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="65" t="str">
+      <c r="D7" s="71">
         <f>IF(Заполнение!D9="","",Заполнение!D9)</f>
-        <v/>
-      </c>
-      <c r="E7" s="65"/>
+        <v>45004</v>
+      </c>
+      <c r="E7" s="71"/>
       <c r="F7" s="24"/>
       <c r="G7" s="26"/>
     </row>
@@ -2757,10 +2796,10 @@
       <c r="C8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="64">
+      <c r="D8" s="70">
         <v>1</v>
       </c>
-      <c r="E8" s="64"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="24"/>
       <c r="G8" s="26"/>
     </row>
@@ -2780,10 +2819,10 @@
       <c r="B10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="71"/>
+      <c r="D10" s="75"/>
       <c r="E10" s="31" t="s">
         <v>6</v>
       </c>
@@ -2800,24 +2839,24 @@
       </c>
       <c r="B11" s="34" t="str">
         <f>IF(Заполнение!C13="","",Заполнение!C13)</f>
-        <v/>
-      </c>
-      <c r="C11" s="72" t="str">
+        <v>asdf</v>
+      </c>
+      <c r="C11" s="76" t="str">
         <f>IF(Заполнение!D13="","",Заполнение!D13)</f>
-        <v/>
-      </c>
-      <c r="D11" s="73"/>
+        <v>dsa</v>
+      </c>
+      <c r="D11" s="77"/>
       <c r="E11" s="35" t="str">
         <f>IF(Заполнение!E13="","",Заполнение!E13)</f>
-        <v/>
+        <v>sd</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>IF(Заполнение!F13="","",Заполнение!F13)</f>
-        <v/>
-      </c>
-      <c r="G11" s="33" t="str">
+        <v>Главный судья соревнований</v>
+      </c>
+      <c r="G11" s="33">
         <f>IF(Заполнение!H13="","",Заполнение!H13)</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2829,11 +2868,11 @@
         <f>IF(Заполнение!C14="","",Заполнение!C14)</f>
         <v/>
       </c>
-      <c r="C12" s="68" t="str">
+      <c r="C12" s="66" t="str">
         <f>IF(Заполнение!D14="","",Заполнение!D14)</f>
         <v/>
       </c>
-      <c r="D12" s="69"/>
+      <c r="D12" s="67"/>
       <c r="E12" s="35" t="str">
         <f>IF(Заполнение!E14="","",Заполнение!E14)</f>
         <v/>
@@ -2856,11 +2895,11 @@
         <f>IF(Заполнение!C15="","",Заполнение!C15)</f>
         <v/>
       </c>
-      <c r="C13" s="68" t="str">
+      <c r="C13" s="66" t="str">
         <f>IF(Заполнение!D15="","",Заполнение!D15)</f>
         <v/>
       </c>
-      <c r="D13" s="69"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="35" t="str">
         <f>IF(Заполнение!E15="","",Заполнение!E15)</f>
         <v/>
@@ -2883,11 +2922,11 @@
         <f>IF(Заполнение!C16="","",Заполнение!C16)</f>
         <v/>
       </c>
-      <c r="C14" s="68" t="str">
+      <c r="C14" s="66" t="str">
         <f>IF(Заполнение!D16="","",Заполнение!D16)</f>
         <v/>
       </c>
-      <c r="D14" s="69"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="35" t="str">
         <f>IF(Заполнение!E16="","",Заполнение!E16)</f>
         <v/>
@@ -2910,11 +2949,11 @@
         <f>IF(Заполнение!C17="","",Заполнение!C17)</f>
         <v/>
       </c>
-      <c r="C15" s="68" t="str">
+      <c r="C15" s="66" t="str">
         <f>IF(Заполнение!D17="","",Заполнение!D17)</f>
         <v/>
       </c>
-      <c r="D15" s="69"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="35" t="str">
         <f>IF(Заполнение!E17="","",Заполнение!E17)</f>
         <v/>
@@ -2937,11 +2976,11 @@
         <f>IF(Заполнение!C18="","",Заполнение!C18)</f>
         <v/>
       </c>
-      <c r="C16" s="68" t="str">
+      <c r="C16" s="66" t="str">
         <f>IF(Заполнение!D18="","",Заполнение!D18)</f>
         <v/>
       </c>
-      <c r="D16" s="69"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="35" t="str">
         <f>IF(Заполнение!E18="","",Заполнение!E18)</f>
         <v/>
@@ -2964,11 +3003,11 @@
         <f>IF(Заполнение!C19="","",Заполнение!C19)</f>
         <v/>
       </c>
-      <c r="C17" s="68" t="str">
+      <c r="C17" s="66" t="str">
         <f>IF(Заполнение!D19="","",Заполнение!D19)</f>
         <v/>
       </c>
-      <c r="D17" s="69"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="35" t="str">
         <f>IF(Заполнение!E19="","",Заполнение!E19)</f>
         <v/>
@@ -2991,11 +3030,11 @@
         <f>IF(Заполнение!C20="","",Заполнение!C20)</f>
         <v/>
       </c>
-      <c r="C18" s="68" t="str">
+      <c r="C18" s="66" t="str">
         <f>IF(Заполнение!D20="","",Заполнение!D20)</f>
         <v/>
       </c>
-      <c r="D18" s="69"/>
+      <c r="D18" s="67"/>
       <c r="E18" s="35" t="str">
         <f>IF(Заполнение!E20="","",Заполнение!E20)</f>
         <v/>
@@ -3018,11 +3057,11 @@
         <f>IF(Заполнение!C21="","",Заполнение!C21)</f>
         <v/>
       </c>
-      <c r="C19" s="68" t="str">
+      <c r="C19" s="66" t="str">
         <f>IF(Заполнение!D21="","",Заполнение!D21)</f>
         <v/>
       </c>
-      <c r="D19" s="69"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="35" t="str">
         <f>IF(Заполнение!E21="","",Заполнение!E21)</f>
         <v/>
@@ -3045,11 +3084,11 @@
         <f>IF(Заполнение!C22="","",Заполнение!C22)</f>
         <v/>
       </c>
-      <c r="C20" s="68" t="str">
+      <c r="C20" s="66" t="str">
         <f>IF(Заполнение!D22="","",Заполнение!D22)</f>
         <v/>
       </c>
-      <c r="D20" s="69"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="35" t="str">
         <f>IF(Заполнение!E22="","",Заполнение!E22)</f>
         <v/>
@@ -3072,11 +3111,11 @@
         <f>IF(Заполнение!C23="","",Заполнение!C23)</f>
         <v/>
       </c>
-      <c r="C21" s="68" t="str">
+      <c r="C21" s="66" t="str">
         <f>IF(Заполнение!D23="","",Заполнение!D23)</f>
         <v/>
       </c>
-      <c r="D21" s="69"/>
+      <c r="D21" s="67"/>
       <c r="E21" s="35" t="str">
         <f>IF(Заполнение!E23="","",Заполнение!E23)</f>
         <v/>
@@ -3099,11 +3138,11 @@
         <f>IF(Заполнение!C24="","",Заполнение!C24)</f>
         <v/>
       </c>
-      <c r="C22" s="68" t="str">
+      <c r="C22" s="66" t="str">
         <f>IF(Заполнение!D24="","",Заполнение!D24)</f>
         <v/>
       </c>
-      <c r="D22" s="69"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="35" t="str">
         <f>IF(Заполнение!E24="","",Заполнение!E24)</f>
         <v/>
@@ -3126,11 +3165,11 @@
         <f>IF(Заполнение!C25="","",Заполнение!C25)</f>
         <v/>
       </c>
-      <c r="C23" s="68" t="str">
+      <c r="C23" s="66" t="str">
         <f>IF(Заполнение!D25="","",Заполнение!D25)</f>
         <v/>
       </c>
-      <c r="D23" s="69"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="35" t="str">
         <f>IF(Заполнение!E25="","",Заполнение!E25)</f>
         <v/>
@@ -3153,11 +3192,11 @@
         <f>IF(Заполнение!C26="","",Заполнение!C26)</f>
         <v/>
       </c>
-      <c r="C24" s="68" t="str">
+      <c r="C24" s="66" t="str">
         <f>IF(Заполнение!D26="","",Заполнение!D26)</f>
         <v/>
       </c>
-      <c r="D24" s="69"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="35" t="str">
         <f>IF(Заполнение!E26="","",Заполнение!E26)</f>
         <v/>
@@ -3180,11 +3219,11 @@
         <f>IF(Заполнение!C27="","",Заполнение!C27)</f>
         <v/>
       </c>
-      <c r="C25" s="68" t="str">
+      <c r="C25" s="66" t="str">
         <f>IF(Заполнение!D27="","",Заполнение!D27)</f>
         <v/>
       </c>
-      <c r="D25" s="69"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="35" t="str">
         <f>IF(Заполнение!E27="","",Заполнение!E27)</f>
         <v/>
@@ -3207,11 +3246,11 @@
         <f>IF(Заполнение!C28="","",Заполнение!C28)</f>
         <v/>
       </c>
-      <c r="C26" s="68" t="str">
+      <c r="C26" s="66" t="str">
         <f>IF(Заполнение!D28="","",Заполнение!D28)</f>
         <v/>
       </c>
-      <c r="D26" s="69"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="35" t="str">
         <f>IF(Заполнение!E28="","",Заполнение!E28)</f>
         <v/>
@@ -3234,11 +3273,11 @@
         <f>IF(Заполнение!C29="","",Заполнение!C29)</f>
         <v/>
       </c>
-      <c r="C27" s="68" t="str">
+      <c r="C27" s="66" t="str">
         <f>IF(Заполнение!D29="","",Заполнение!D29)</f>
         <v/>
       </c>
-      <c r="D27" s="69"/>
+      <c r="D27" s="67"/>
       <c r="E27" s="35" t="str">
         <f>IF(Заполнение!E29="","",Заполнение!E29)</f>
         <v/>
@@ -3261,11 +3300,11 @@
         <f>IF(Заполнение!C30="","",Заполнение!C30)</f>
         <v/>
       </c>
-      <c r="C28" s="68" t="str">
+      <c r="C28" s="66" t="str">
         <f>IF(Заполнение!D30="","",Заполнение!D30)</f>
         <v/>
       </c>
-      <c r="D28" s="69"/>
+      <c r="D28" s="67"/>
       <c r="E28" s="35" t="str">
         <f>IF(Заполнение!E30="","",Заполнение!E30)</f>
         <v/>
@@ -3288,11 +3327,11 @@
         <f>IF(Заполнение!C31="","",Заполнение!C31)</f>
         <v/>
       </c>
-      <c r="C29" s="68" t="str">
+      <c r="C29" s="66" t="str">
         <f>IF(Заполнение!D31="","",Заполнение!D31)</f>
         <v/>
       </c>
-      <c r="D29" s="69"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="35" t="str">
         <f>IF(Заполнение!E31="","",Заполнение!E31)</f>
         <v/>
@@ -3315,11 +3354,11 @@
         <f>IF(Заполнение!C32="","",Заполнение!C32)</f>
         <v/>
       </c>
-      <c r="C30" s="68" t="str">
+      <c r="C30" s="66" t="str">
         <f>IF(Заполнение!D32="","",Заполнение!D32)</f>
         <v/>
       </c>
-      <c r="D30" s="69"/>
+      <c r="D30" s="67"/>
       <c r="E30" s="35" t="str">
         <f>IF(Заполнение!E32="","",Заполнение!E32)</f>
         <v/>
@@ -3342,11 +3381,11 @@
         <f>IF(Заполнение!C33="","",Заполнение!C33)</f>
         <v/>
       </c>
-      <c r="C31" s="68" t="str">
+      <c r="C31" s="66" t="str">
         <f>IF(Заполнение!D33="","",Заполнение!D33)</f>
         <v/>
       </c>
-      <c r="D31" s="69"/>
+      <c r="D31" s="67"/>
       <c r="E31" s="35" t="str">
         <f>IF(Заполнение!E33="","",Заполнение!E33)</f>
         <v/>
@@ -3369,11 +3408,11 @@
         <f>IF(Заполнение!C34="","",Заполнение!C34)</f>
         <v/>
       </c>
-      <c r="C32" s="68" t="str">
+      <c r="C32" s="66" t="str">
         <f>IF(Заполнение!D34="","",Заполнение!D34)</f>
         <v/>
       </c>
-      <c r="D32" s="69"/>
+      <c r="D32" s="67"/>
       <c r="E32" s="35" t="str">
         <f>IF(Заполнение!E34="","",Заполнение!E34)</f>
         <v/>
@@ -3396,11 +3435,11 @@
         <f>IF(Заполнение!C35="","",Заполнение!C35)</f>
         <v/>
       </c>
-      <c r="C33" s="68" t="str">
+      <c r="C33" s="66" t="str">
         <f>IF(Заполнение!D35="","",Заполнение!D35)</f>
         <v/>
       </c>
-      <c r="D33" s="69"/>
+      <c r="D33" s="67"/>
       <c r="E33" s="35" t="str">
         <f>IF(Заполнение!E35="","",Заполнение!E35)</f>
         <v/>
@@ -3423,11 +3462,11 @@
         <f>IF(Заполнение!C36="","",Заполнение!C36)</f>
         <v/>
       </c>
-      <c r="C34" s="68" t="str">
+      <c r="C34" s="66" t="str">
         <f>IF(Заполнение!D36="","",Заполнение!D36)</f>
         <v/>
       </c>
-      <c r="D34" s="69"/>
+      <c r="D34" s="67"/>
       <c r="E34" s="35" t="str">
         <f>IF(Заполнение!E36="","",Заполнение!E36)</f>
         <v/>
@@ -3450,11 +3489,11 @@
         <f>IF(Заполнение!C37="","",Заполнение!C37)</f>
         <v/>
       </c>
-      <c r="C35" s="68" t="str">
+      <c r="C35" s="66" t="str">
         <f>IF(Заполнение!D37="","",Заполнение!D37)</f>
         <v/>
       </c>
-      <c r="D35" s="69"/>
+      <c r="D35" s="67"/>
       <c r="E35" s="35" t="str">
         <f>IF(Заполнение!E37="","",Заполнение!E37)</f>
         <v/>
@@ -3477,11 +3516,11 @@
         <f>IF(Заполнение!C38="","",Заполнение!C38)</f>
         <v/>
       </c>
-      <c r="C36" s="68" t="str">
+      <c r="C36" s="66" t="str">
         <f>IF(Заполнение!D38="","",Заполнение!D38)</f>
         <v/>
       </c>
-      <c r="D36" s="69"/>
+      <c r="D36" s="67"/>
       <c r="E36" s="35" t="str">
         <f>IF(Заполнение!E38="","",Заполнение!E38)</f>
         <v/>
@@ -3504,11 +3543,11 @@
         <f>IF(Заполнение!C39="","",Заполнение!C39)</f>
         <v/>
       </c>
-      <c r="C37" s="68" t="str">
+      <c r="C37" s="66" t="str">
         <f>IF(Заполнение!D39="","",Заполнение!D39)</f>
         <v/>
       </c>
-      <c r="D37" s="69"/>
+      <c r="D37" s="67"/>
       <c r="E37" s="35" t="str">
         <f>IF(Заполнение!E39="","",Заполнение!E39)</f>
         <v/>
@@ -3531,11 +3570,11 @@
         <f>IF(Заполнение!C40="","",Заполнение!C40)</f>
         <v/>
       </c>
-      <c r="C38" s="68" t="str">
+      <c r="C38" s="66" t="str">
         <f>IF(Заполнение!D40="","",Заполнение!D40)</f>
         <v/>
       </c>
-      <c r="D38" s="69"/>
+      <c r="D38" s="67"/>
       <c r="E38" s="35" t="str">
         <f>IF(Заполнение!E40="","",Заполнение!E40)</f>
         <v/>
@@ -3558,11 +3597,11 @@
         <f>IF(Заполнение!C41="","",Заполнение!C41)</f>
         <v/>
       </c>
-      <c r="C39" s="68" t="str">
+      <c r="C39" s="66" t="str">
         <f>IF(Заполнение!D41="","",Заполнение!D41)</f>
         <v/>
       </c>
-      <c r="D39" s="69"/>
+      <c r="D39" s="67"/>
       <c r="E39" s="35" t="str">
         <f>IF(Заполнение!E41="","",Заполнение!E41)</f>
         <v/>
@@ -3585,11 +3624,11 @@
         <f>IF(Заполнение!C42="","",Заполнение!C42)</f>
         <v/>
       </c>
-      <c r="C40" s="68" t="str">
+      <c r="C40" s="66" t="str">
         <f>IF(Заполнение!D42="","",Заполнение!D42)</f>
         <v/>
       </c>
-      <c r="D40" s="69"/>
+      <c r="D40" s="67"/>
       <c r="E40" s="35" t="str">
         <f>IF(Заполнение!E42="","",Заполнение!E42)</f>
         <v/>
@@ -3612,11 +3651,11 @@
         <f>IF(Заполнение!C43="","",Заполнение!C43)</f>
         <v/>
       </c>
-      <c r="C41" s="68" t="str">
+      <c r="C41" s="66" t="str">
         <f>IF(Заполнение!D43="","",Заполнение!D43)</f>
         <v/>
       </c>
-      <c r="D41" s="69"/>
+      <c r="D41" s="67"/>
       <c r="E41" s="35" t="str">
         <f>IF(Заполнение!E43="","",Заполнение!E43)</f>
         <v/>
@@ -3639,11 +3678,11 @@
         <f>IF(Заполнение!C44="","",Заполнение!C44)</f>
         <v/>
       </c>
-      <c r="C42" s="68" t="str">
+      <c r="C42" s="66" t="str">
         <f>IF(Заполнение!D44="","",Заполнение!D44)</f>
         <v/>
       </c>
-      <c r="D42" s="69"/>
+      <c r="D42" s="67"/>
       <c r="E42" s="35" t="str">
         <f>IF(Заполнение!E44="","",Заполнение!E44)</f>
         <v/>
@@ -3666,11 +3705,11 @@
         <f>IF(Заполнение!C45="","",Заполнение!C45)</f>
         <v/>
       </c>
-      <c r="C43" s="68" t="str">
+      <c r="C43" s="66" t="str">
         <f>IF(Заполнение!D45="","",Заполнение!D45)</f>
         <v/>
       </c>
-      <c r="D43" s="69"/>
+      <c r="D43" s="67"/>
       <c r="E43" s="35" t="str">
         <f>IF(Заполнение!E45="","",Заполнение!E45)</f>
         <v/>
@@ -3693,11 +3732,11 @@
         <f>IF(Заполнение!C46="","",Заполнение!C46)</f>
         <v/>
       </c>
-      <c r="C44" s="68" t="str">
+      <c r="C44" s="66" t="str">
         <f>IF(Заполнение!D46="","",Заполнение!D46)</f>
         <v/>
       </c>
-      <c r="D44" s="69"/>
+      <c r="D44" s="67"/>
       <c r="E44" s="35" t="str">
         <f>IF(Заполнение!E46="","",Заполнение!E46)</f>
         <v/>
@@ -3720,11 +3759,11 @@
         <f>IF(Заполнение!C47="","",Заполнение!C47)</f>
         <v/>
       </c>
-      <c r="C45" s="68" t="str">
+      <c r="C45" s="66" t="str">
         <f>IF(Заполнение!D47="","",Заполнение!D47)</f>
         <v/>
       </c>
-      <c r="D45" s="69"/>
+      <c r="D45" s="67"/>
       <c r="E45" s="35" t="str">
         <f>IF(Заполнение!E47="","",Заполнение!E47)</f>
         <v/>
@@ -3747,11 +3786,11 @@
         <f>IF(Заполнение!C48="","",Заполнение!C48)</f>
         <v/>
       </c>
-      <c r="C46" s="68" t="str">
+      <c r="C46" s="66" t="str">
         <f>IF(Заполнение!D48="","",Заполнение!D48)</f>
         <v/>
       </c>
-      <c r="D46" s="69"/>
+      <c r="D46" s="67"/>
       <c r="E46" s="35" t="str">
         <f>IF(Заполнение!E48="","",Заполнение!E48)</f>
         <v/>
@@ -3774,11 +3813,11 @@
         <f>IF(Заполнение!C49="","",Заполнение!C49)</f>
         <v/>
       </c>
-      <c r="C47" s="68" t="str">
+      <c r="C47" s="66" t="str">
         <f>IF(Заполнение!D49="","",Заполнение!D49)</f>
         <v/>
       </c>
-      <c r="D47" s="69"/>
+      <c r="D47" s="67"/>
       <c r="E47" s="35" t="str">
         <f>IF(Заполнение!E49="","",Заполнение!E49)</f>
         <v/>
@@ -3801,11 +3840,11 @@
         <f>IF(Заполнение!C50="","",Заполнение!C50)</f>
         <v/>
       </c>
-      <c r="C48" s="75" t="str">
+      <c r="C48" s="68" t="str">
         <f>IF(Заполнение!D50="","",Заполнение!D50)</f>
         <v/>
       </c>
-      <c r="D48" s="76"/>
+      <c r="D48" s="69"/>
       <c r="E48" s="39" t="str">
         <f>IF(Заполнение!E50="","",Заполнение!E50)</f>
         <v/>
@@ -3820,307 +3859,307 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C49" s="74"/>
-      <c r="D49" s="74"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64"/>
       <c r="G49" s="23"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="66"/>
-      <c r="C51" s="66"/>
-      <c r="D51" s="66"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="67" t="s">
+      <c r="B51" s="72"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="G51" s="67"/>
+      <c r="G51" s="73"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="66"/>
-      <c r="B52" s="66"/>
-      <c r="C52" s="66"/>
-      <c r="D52" s="66"/>
-      <c r="E52" s="66"/>
-      <c r="F52" s="67" t="s">
+      <c r="A52" s="72"/>
+      <c r="B52" s="72"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="G52" s="67"/>
+      <c r="G52" s="73"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="66"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="66"/>
-      <c r="E53" s="66"/>
-      <c r="F53" s="67" t="str">
+      <c r="B53" s="72"/>
+      <c r="C53" s="72"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="72"/>
+      <c r="F53" s="73" t="str">
         <f ca="1">"Дата: " &amp; TEXT(TODAY(),"ДД.ММ.ГГГГ")</f>
-        <v>Дата: 03.03.2023</v>
-      </c>
-      <c r="G53" s="67"/>
+        <v>Дата: 19.03.2023</v>
+      </c>
+      <c r="G53" s="73"/>
       <c r="I53" s="46"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
+      <c r="C54" s="64"/>
+      <c r="D54" s="64"/>
       <c r="G54" s="23"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="74"/>
-      <c r="D55" s="74"/>
+      <c r="C55" s="64"/>
+      <c r="D55" s="64"/>
       <c r="G55" s="23"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="74"/>
-      <c r="D56" s="74"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="64"/>
       <c r="G56" s="23"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="74"/>
-      <c r="D57" s="74"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="64"/>
       <c r="G57" s="23"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="74"/>
-      <c r="D58" s="74"/>
+      <c r="C58" s="64"/>
+      <c r="D58" s="64"/>
       <c r="G58" s="23"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="74"/>
-      <c r="D62" s="74"/>
+      <c r="C62" s="64"/>
+      <c r="D62" s="64"/>
       <c r="G62" s="23"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="74"/>
-      <c r="D63" s="74"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="64"/>
       <c r="G63" s="23"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C64" s="74"/>
-      <c r="D64" s="74"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="64"/>
       <c r="G64" s="23"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="74"/>
-      <c r="D65" s="74"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="64"/>
       <c r="G65" s="23"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="74"/>
-      <c r="D66" s="74"/>
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
       <c r="G66" s="23"/>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="74"/>
-      <c r="D67" s="74"/>
+      <c r="C67" s="64"/>
+      <c r="D67" s="64"/>
       <c r="G67" s="23"/>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="74"/>
-      <c r="D68" s="74"/>
+      <c r="C68" s="64"/>
+      <c r="D68" s="64"/>
       <c r="G68" s="23"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="74"/>
-      <c r="D69" s="74"/>
+      <c r="C69" s="64"/>
+      <c r="D69" s="64"/>
       <c r="G69" s="23"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
+      <c r="C70" s="64"/>
+      <c r="D70" s="64"/>
       <c r="G70" s="23"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="74"/>
-      <c r="D71" s="74"/>
+      <c r="C71" s="64"/>
+      <c r="D71" s="64"/>
       <c r="G71" s="23"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="74"/>
-      <c r="D72" s="74"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
       <c r="G72" s="23"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="74"/>
-      <c r="D73" s="74"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
       <c r="G73" s="23"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
       <c r="G74" s="23"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="74"/>
-      <c r="D75" s="74"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64"/>
       <c r="G75" s="23"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="74"/>
-      <c r="D76" s="74"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64"/>
       <c r="G76" s="23"/>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="74"/>
-      <c r="D77" s="74"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="64"/>
       <c r="G77" s="23"/>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="74"/>
-      <c r="D78" s="74"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="64"/>
       <c r="G78" s="23"/>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="74"/>
-      <c r="D79" s="74"/>
+      <c r="C79" s="64"/>
+      <c r="D79" s="64"/>
       <c r="G79" s="23"/>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="74"/>
-      <c r="D80" s="74"/>
+      <c r="C80" s="64"/>
+      <c r="D80" s="64"/>
       <c r="G80" s="23"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="74"/>
-      <c r="D81" s="74"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="64"/>
       <c r="G81" s="23"/>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="74"/>
-      <c r="D82" s="74"/>
+      <c r="C82" s="64"/>
+      <c r="D82" s="64"/>
       <c r="G82" s="23"/>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="74"/>
-      <c r="D83" s="74"/>
+      <c r="C83" s="64"/>
+      <c r="D83" s="64"/>
       <c r="G83" s="23"/>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="74"/>
-      <c r="D84" s="74"/>
+      <c r="C84" s="64"/>
+      <c r="D84" s="64"/>
       <c r="G84" s="23"/>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="74"/>
-      <c r="D85" s="74"/>
+      <c r="C85" s="64"/>
+      <c r="D85" s="64"/>
       <c r="G85" s="23"/>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="74"/>
-      <c r="D86" s="74"/>
+      <c r="C86" s="64"/>
+      <c r="D86" s="64"/>
       <c r="G86" s="23"/>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="74"/>
-      <c r="D87" s="74"/>
+      <c r="C87" s="64"/>
+      <c r="D87" s="64"/>
       <c r="G87" s="23"/>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="74"/>
-      <c r="D88" s="74"/>
+      <c r="C88" s="64"/>
+      <c r="D88" s="64"/>
       <c r="G88" s="23"/>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="74"/>
-      <c r="D89" s="74"/>
+      <c r="C89" s="64"/>
+      <c r="D89" s="64"/>
       <c r="G89" s="23"/>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="74"/>
-      <c r="D90" s="74"/>
+      <c r="C90" s="64"/>
+      <c r="D90" s="64"/>
       <c r="G90" s="23"/>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="74"/>
-      <c r="D91" s="74"/>
+      <c r="C91" s="64"/>
+      <c r="D91" s="64"/>
       <c r="G91" s="23"/>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="74"/>
-      <c r="D92" s="74"/>
+      <c r="C92" s="64"/>
+      <c r="D92" s="64"/>
       <c r="G92" s="23"/>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="74"/>
-      <c r="D93" s="74"/>
+      <c r="C93" s="64"/>
+      <c r="D93" s="64"/>
       <c r="G93" s="23"/>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="74"/>
-      <c r="D94" s="74"/>
+      <c r="C94" s="64"/>
+      <c r="D94" s="64"/>
       <c r="G94" s="23"/>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C95" s="74"/>
-      <c r="D95" s="74"/>
+      <c r="C95" s="64"/>
+      <c r="D95" s="64"/>
       <c r="G95" s="23"/>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C96" s="74"/>
-      <c r="D96" s="74"/>
+      <c r="C96" s="64"/>
+      <c r="D96" s="64"/>
       <c r="G96" s="23"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C97" s="74"/>
-      <c r="D97" s="74"/>
+      <c r="C97" s="64"/>
+      <c r="D97" s="64"/>
       <c r="G97" s="23"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C98" s="74"/>
-      <c r="D98" s="74"/>
+      <c r="C98" s="64"/>
+      <c r="D98" s="64"/>
       <c r="G98" s="23"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C99" s="74"/>
-      <c r="D99" s="74"/>
+      <c r="C99" s="64"/>
+      <c r="D99" s="64"/>
       <c r="G99" s="23"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C100" s="74"/>
-      <c r="D100" s="74"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="64"/>
       <c r="G100" s="23"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C101" s="74"/>
-      <c r="D101" s="74"/>
+      <c r="C101" s="64"/>
+      <c r="D101" s="64"/>
       <c r="G101" s="23"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C102" s="74"/>
-      <c r="D102" s="74"/>
+      <c r="C102" s="64"/>
+      <c r="D102" s="64"/>
       <c r="G102" s="23"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C103" s="74"/>
-      <c r="D103" s="74"/>
+      <c r="C103" s="64"/>
+      <c r="D103" s="64"/>
       <c r="G103" s="23"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C104" s="74"/>
-      <c r="D104" s="74"/>
+      <c r="C104" s="64"/>
+      <c r="D104" s="64"/>
       <c r="G104" s="23"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C105" s="74"/>
-      <c r="D105" s="74"/>
+      <c r="C105" s="64"/>
+      <c r="D105" s="64"/>
       <c r="G105" s="23"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C106" s="74"/>
-      <c r="D106" s="74"/>
+      <c r="C106" s="64"/>
+      <c r="D106" s="64"/>
       <c r="G106" s="23"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C107" s="74"/>
-      <c r="D107" s="74"/>
+      <c r="C107" s="64"/>
+      <c r="D107" s="64"/>
       <c r="G107" s="23"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C108" s="74"/>
-      <c r="D108" s="74"/>
+      <c r="C108" s="64"/>
+      <c r="D108" s="64"/>
       <c r="G108" s="23"/>
     </row>
     <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -4136,6 +4175,83 @@
     </row>
   </sheetData>
   <mergeCells count="101">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
     <mergeCell ref="C107:D107"/>
     <mergeCell ref="C108:D108"/>
     <mergeCell ref="A1:G3"/>
@@ -4160,83 +4276,6 @@
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="C91:D91"/>
     <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
feat: add list of referees to second sheet of New Referee template
</commit_message>
<xml_diff>
--- a/Resources/Template_Competition.xlsx
+++ b/Resources/Template_Competition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A28D91-933E-4BA9-B642-3C71A293A407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC92474-227D-4819-B4D8-4FC0F1A94525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Заполнение" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Название соревнования:</t>
   </si>
@@ -84,30 +84,6 @@
   </si>
   <si>
     <t>Должность</t>
-  </si>
-  <si>
-    <t>Пояснение к цветовым обозначениям ячейки:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Обязательно для заполнения</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Допустимо для заполнения</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Не для редактирования *белый цвет* </t>
-  </si>
-  <si>
-    <t>Успех ✓</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Ответ бота на правильно заполненные данные (Не для редактирования)</t>
-  </si>
-  <si>
-    <t>Ошибка</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Ответ бота на неправильно заполненные данные (Не для редактирования)</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -153,9 +129,6 @@
     <t>Неизвестно</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Пример оформления даты</t>
-  </si>
-  <si>
     <t>Гонтаренко И.А.</t>
   </si>
   <si>
@@ -167,18 +140,6 @@
   <si>
     <t>Данные о судейской бригаде, участвовавшей в соревновании.
 Для формирования рейтинга в учетной базе FEMIDA</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>dsa</t>
-  </si>
-  <si>
-    <t>sd</t>
   </si>
 </sst>
 </file>
@@ -263,7 +224,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,12 +234,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -652,18 +607,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -671,55 +614,55 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -733,9 +676,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -744,7 +684,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -787,43 +727,43 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1226,7 +1166,7 @@
   <dimension ref="B1:Z111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,81 +1176,69 @@
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="56" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="51" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" customWidth="1"/>
     <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B1" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
       <c r="Z2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="W3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="K3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="W3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="51"/>
+      <c r="G4" s="46"/>
       <c r="H4" s="1"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="W4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="51"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="1"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="W5" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1319,14 +1247,10 @@
       <c r="D6" s="3"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="51"/>
+      <c r="G6" s="46"/>
       <c r="H6" s="1"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="W6" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1334,21 +1258,13 @@
       <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="60"/>
-      <c r="K7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D7" s="53"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="55"/>
       <c r="W7" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1356,21 +1272,13 @@
       <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="60"/>
-      <c r="K8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55"/>
       <c r="W8" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1378,16 +1286,13 @@
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="61">
-        <v>45004</v>
-      </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="63"/>
-      <c r="K9" s="2"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="58"/>
       <c r="W9" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -1396,23 +1301,16 @@
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="51"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="1"/>
-      <c r="K10" s="45">
-        <f ca="1">TODAY()</f>
-        <v>45004</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:26" s="50" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:26" s="45" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="52"/>
+      <c r="G11" s="47"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1433,37 +1331,25 @@
         <v>6</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="53" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>1</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="47">
-        <v>1</v>
-      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="42"/>
     </row>
     <row r="14" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="str">
@@ -1474,8 +1360,8 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="47"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="42"/>
     </row>
     <row r="15" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="str">
@@ -1486,9 +1372,9 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="47"/>
-      <c r="J15" s="56"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="42"/>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="str">
@@ -1499,8 +1385,8 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="47"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="42"/>
     </row>
     <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="str">
@@ -1511,9 +1397,9 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="47"/>
-      <c r="J17" s="56"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="42"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="str">
@@ -1524,8 +1410,8 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="47"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="42"/>
     </row>
     <row r="19" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="str">
@@ -1536,8 +1422,8 @@
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="47"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="42"/>
     </row>
     <row r="20" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="str">
@@ -1548,8 +1434,8 @@
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="47"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="42"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1561,8 +1447,8 @@
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="47"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="42"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1574,8 +1460,8 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="47"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="42"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1587,8 +1473,8 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="47"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="42"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1600,8 +1486,8 @@
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="47"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="42"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1613,8 +1499,8 @@
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="47"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="42"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1626,8 +1512,8 @@
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="47"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="42"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1639,8 +1525,8 @@
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="47"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="42"/>
     </row>
     <row r="28" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="str">
@@ -1651,8 +1537,8 @@
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="47"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="42"/>
     </row>
     <row r="29" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="str">
@@ -1663,8 +1549,8 @@
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="47"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="42"/>
     </row>
     <row r="30" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="str">
@@ -1675,8 +1561,8 @@
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="47"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="42"/>
     </row>
     <row r="31" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="str">
@@ -1687,8 +1573,8 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="47"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="42"/>
     </row>
     <row r="32" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="str">
@@ -1699,8 +1585,8 @@
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="47"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="42"/>
     </row>
     <row r="33" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="str">
@@ -1711,8 +1597,8 @@
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="13"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="47"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="42"/>
     </row>
     <row r="34" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="str">
@@ -1723,8 +1609,8 @@
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="47"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="42"/>
     </row>
     <row r="35" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="str">
@@ -1735,8 +1621,8 @@
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="47"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="42"/>
     </row>
     <row r="36" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="str">
@@ -1747,8 +1633,8 @@
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="47"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="42"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="str">
@@ -1759,8 +1645,8 @@
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="47"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="42"/>
     </row>
     <row r="38" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="str">
@@ -1771,8 +1657,8 @@
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="47"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="42"/>
     </row>
     <row r="39" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="str">
@@ -1783,8 +1669,8 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="47"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="42"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="str">
@@ -1795,8 +1681,8 @@
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="13"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="47"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="42"/>
     </row>
     <row r="41" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="str">
@@ -1807,8 +1693,8 @@
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="13"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="47"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="42"/>
     </row>
     <row r="42" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="str">
@@ -1819,8 +1705,8 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="13"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="47"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="42"/>
     </row>
     <row r="43" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="str">
@@ -1831,8 +1717,8 @@
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="13"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="47"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="42"/>
     </row>
     <row r="44" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="str">
@@ -1843,8 +1729,8 @@
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="13"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="47"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="42"/>
     </row>
     <row r="45" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="str">
@@ -1855,8 +1741,8 @@
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="13"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="47"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="42"/>
     </row>
     <row r="46" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="str">
@@ -1867,8 +1753,8 @@
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="13"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="47"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="42"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="str">
@@ -1879,8 +1765,8 @@
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="13"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="47"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="42"/>
     </row>
     <row r="48" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="str">
@@ -1891,8 +1777,8 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="13"/>
-      <c r="G48" s="54"/>
-      <c r="H48" s="47"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="42"/>
     </row>
     <row r="49" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="str">
@@ -1903,8 +1789,8 @@
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="13"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="47"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="42"/>
     </row>
     <row r="50" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="str">
@@ -1915,8 +1801,8 @@
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="13"/>
-      <c r="G50" s="54"/>
-      <c r="H50" s="47"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="42"/>
     </row>
     <row r="51" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="str">
@@ -1927,8 +1813,8 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="13"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="47"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="42"/>
     </row>
     <row r="52" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="str">
@@ -1939,8 +1825,8 @@
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="13"/>
-      <c r="G52" s="54"/>
-      <c r="H52" s="47"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="42"/>
     </row>
     <row r="53" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="str">
@@ -1951,8 +1837,8 @@
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="13"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="47"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="42"/>
     </row>
     <row r="54" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="str">
@@ -1963,8 +1849,8 @@
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="13"/>
-      <c r="G54" s="54"/>
-      <c r="H54" s="47"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="42"/>
     </row>
     <row r="55" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="str">
@@ -1975,8 +1861,8 @@
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="13"/>
-      <c r="G55" s="54"/>
-      <c r="H55" s="47"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="42"/>
     </row>
     <row r="56" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="str">
@@ -1987,8 +1873,8 @@
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="13"/>
-      <c r="G56" s="54"/>
-      <c r="H56" s="47"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="42"/>
     </row>
     <row r="57" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="str">
@@ -1999,8 +1885,8 @@
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="13"/>
-      <c r="G57" s="54"/>
-      <c r="H57" s="47"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="42"/>
     </row>
     <row r="58" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="str">
@@ -2011,8 +1897,8 @@
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="13"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="47"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="42"/>
     </row>
     <row r="59" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="str">
@@ -2023,8 +1909,8 @@
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="13"/>
-      <c r="G59" s="54"/>
-      <c r="H59" s="47"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="42"/>
     </row>
     <row r="60" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="str">
@@ -2035,8 +1921,8 @@
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="13"/>
-      <c r="G60" s="54"/>
-      <c r="H60" s="47"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="42"/>
     </row>
     <row r="61" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="10" t="str">
@@ -2047,8 +1933,8 @@
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
       <c r="F61" s="13"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="47"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="42"/>
     </row>
     <row r="62" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="10" t="str">
@@ -2059,8 +1945,8 @@
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
       <c r="F62" s="13"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="47"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="42"/>
     </row>
     <row r="63" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="str">
@@ -2071,8 +1957,8 @@
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="13"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="47"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="42"/>
     </row>
     <row r="64" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="str">
@@ -2083,8 +1969,8 @@
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
       <c r="F64" s="13"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="47"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="42"/>
     </row>
     <row r="65" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="str">
@@ -2095,8 +1981,8 @@
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
       <c r="F65" s="13"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="47"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="42"/>
     </row>
     <row r="66" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="str">
@@ -2107,8 +1993,8 @@
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
       <c r="F66" s="13"/>
-      <c r="G66" s="54"/>
-      <c r="H66" s="47"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="42"/>
     </row>
     <row r="67" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="10" t="str">
@@ -2119,8 +2005,8 @@
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
       <c r="F67" s="13"/>
-      <c r="G67" s="54"/>
-      <c r="H67" s="47"/>
+      <c r="G67" s="49"/>
+      <c r="H67" s="42"/>
     </row>
     <row r="68" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="str">
@@ -2131,8 +2017,8 @@
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
       <c r="F68" s="13"/>
-      <c r="G68" s="54"/>
-      <c r="H68" s="47"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="42"/>
     </row>
     <row r="69" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="str">
@@ -2143,8 +2029,8 @@
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
       <c r="F69" s="13"/>
-      <c r="G69" s="54"/>
-      <c r="H69" s="47"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="42"/>
     </row>
     <row r="70" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="str">
@@ -2155,8 +2041,8 @@
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
       <c r="F70" s="13"/>
-      <c r="G70" s="54"/>
-      <c r="H70" s="47"/>
+      <c r="G70" s="49"/>
+      <c r="H70" s="42"/>
     </row>
     <row r="71" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="str">
@@ -2167,8 +2053,8 @@
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
       <c r="F71" s="13"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="47"/>
+      <c r="G71" s="49"/>
+      <c r="H71" s="42"/>
     </row>
     <row r="72" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="10" t="str">
@@ -2179,8 +2065,8 @@
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
       <c r="F72" s="13"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="47"/>
+      <c r="G72" s="49"/>
+      <c r="H72" s="42"/>
     </row>
     <row r="73" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="10" t="str">
@@ -2191,8 +2077,8 @@
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="13"/>
-      <c r="G73" s="54"/>
-      <c r="H73" s="47"/>
+      <c r="G73" s="49"/>
+      <c r="H73" s="42"/>
     </row>
     <row r="74" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="10" t="str">
@@ -2203,8 +2089,8 @@
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
       <c r="F74" s="13"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="47"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="42"/>
     </row>
     <row r="75" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B75" s="10" t="str">
@@ -2215,8 +2101,8 @@
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
       <c r="F75" s="13"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="47"/>
+      <c r="G75" s="49"/>
+      <c r="H75" s="42"/>
     </row>
     <row r="76" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B76" s="10" t="str">
@@ -2227,8 +2113,8 @@
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
       <c r="F76" s="13"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="47"/>
+      <c r="G76" s="49"/>
+      <c r="H76" s="42"/>
     </row>
     <row r="77" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B77" s="10" t="str">
@@ -2239,8 +2125,8 @@
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
       <c r="F77" s="13"/>
-      <c r="G77" s="54"/>
-      <c r="H77" s="47"/>
+      <c r="G77" s="49"/>
+      <c r="H77" s="42"/>
     </row>
     <row r="78" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B78" s="10" t="str">
@@ -2251,8 +2137,8 @@
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
       <c r="F78" s="13"/>
-      <c r="G78" s="54"/>
-      <c r="H78" s="47"/>
+      <c r="G78" s="49"/>
+      <c r="H78" s="42"/>
     </row>
     <row r="79" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="str">
@@ -2263,8 +2149,8 @@
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
       <c r="F79" s="13"/>
-      <c r="G79" s="54"/>
-      <c r="H79" s="47"/>
+      <c r="G79" s="49"/>
+      <c r="H79" s="42"/>
     </row>
     <row r="80" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B80" s="10" t="str">
@@ -2275,8 +2161,8 @@
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
       <c r="F80" s="13"/>
-      <c r="G80" s="54"/>
-      <c r="H80" s="47"/>
+      <c r="G80" s="49"/>
+      <c r="H80" s="42"/>
     </row>
     <row r="81" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="str">
@@ -2287,8 +2173,8 @@
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
       <c r="F81" s="13"/>
-      <c r="G81" s="54"/>
-      <c r="H81" s="47"/>
+      <c r="G81" s="49"/>
+      <c r="H81" s="42"/>
     </row>
     <row r="82" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B82" s="10" t="str">
@@ -2299,8 +2185,8 @@
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
       <c r="F82" s="13"/>
-      <c r="G82" s="54"/>
-      <c r="H82" s="47"/>
+      <c r="G82" s="49"/>
+      <c r="H82" s="42"/>
     </row>
     <row r="83" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="10" t="str">
@@ -2311,8 +2197,8 @@
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
       <c r="F83" s="13"/>
-      <c r="G83" s="54"/>
-      <c r="H83" s="47"/>
+      <c r="G83" s="49"/>
+      <c r="H83" s="42"/>
     </row>
     <row r="84" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B84" s="10" t="str">
@@ -2323,8 +2209,8 @@
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
       <c r="F84" s="13"/>
-      <c r="G84" s="54"/>
-      <c r="H84" s="47"/>
+      <c r="G84" s="49"/>
+      <c r="H84" s="42"/>
     </row>
     <row r="85" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B85" s="10" t="str">
@@ -2335,8 +2221,8 @@
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
       <c r="F85" s="13"/>
-      <c r="G85" s="54"/>
-      <c r="H85" s="47"/>
+      <c r="G85" s="49"/>
+      <c r="H85" s="42"/>
     </row>
     <row r="86" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B86" s="10" t="str">
@@ -2347,8 +2233,8 @@
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
       <c r="F86" s="13"/>
-      <c r="G86" s="54"/>
-      <c r="H86" s="47"/>
+      <c r="G86" s="49"/>
+      <c r="H86" s="42"/>
     </row>
     <row r="87" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B87" s="10" t="str">
@@ -2359,8 +2245,8 @@
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
       <c r="F87" s="13"/>
-      <c r="G87" s="54"/>
-      <c r="H87" s="47"/>
+      <c r="G87" s="49"/>
+      <c r="H87" s="42"/>
     </row>
     <row r="88" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B88" s="10" t="str">
@@ -2371,8 +2257,8 @@
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
       <c r="F88" s="13"/>
-      <c r="G88" s="54"/>
-      <c r="H88" s="47"/>
+      <c r="G88" s="49"/>
+      <c r="H88" s="42"/>
     </row>
     <row r="89" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B89" s="10" t="str">
@@ -2383,8 +2269,8 @@
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
       <c r="F89" s="13"/>
-      <c r="G89" s="54"/>
-      <c r="H89" s="47"/>
+      <c r="G89" s="49"/>
+      <c r="H89" s="42"/>
     </row>
     <row r="90" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B90" s="10" t="str">
@@ -2395,8 +2281,8 @@
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
       <c r="F90" s="13"/>
-      <c r="G90" s="54"/>
-      <c r="H90" s="47"/>
+      <c r="G90" s="49"/>
+      <c r="H90" s="42"/>
     </row>
     <row r="91" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B91" s="10" t="str">
@@ -2407,8 +2293,8 @@
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
       <c r="F91" s="13"/>
-      <c r="G91" s="54"/>
-      <c r="H91" s="47"/>
+      <c r="G91" s="49"/>
+      <c r="H91" s="42"/>
     </row>
     <row r="92" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B92" s="10" t="str">
@@ -2419,8 +2305,8 @@
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
       <c r="F92" s="13"/>
-      <c r="G92" s="54"/>
-      <c r="H92" s="47"/>
+      <c r="G92" s="49"/>
+      <c r="H92" s="42"/>
     </row>
     <row r="93" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B93" s="10" t="str">
@@ -2431,8 +2317,8 @@
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
       <c r="F93" s="13"/>
-      <c r="G93" s="54"/>
-      <c r="H93" s="47"/>
+      <c r="G93" s="49"/>
+      <c r="H93" s="42"/>
     </row>
     <row r="94" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B94" s="10" t="str">
@@ -2443,8 +2329,8 @@
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
       <c r="F94" s="13"/>
-      <c r="G94" s="54"/>
-      <c r="H94" s="47"/>
+      <c r="G94" s="49"/>
+      <c r="H94" s="42"/>
     </row>
     <row r="95" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B95" s="10" t="str">
@@ -2455,8 +2341,8 @@
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
       <c r="F95" s="13"/>
-      <c r="G95" s="54"/>
-      <c r="H95" s="47"/>
+      <c r="G95" s="49"/>
+      <c r="H95" s="42"/>
     </row>
     <row r="96" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B96" s="10" t="str">
@@ -2467,8 +2353,8 @@
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
       <c r="F96" s="13"/>
-      <c r="G96" s="54"/>
-      <c r="H96" s="47"/>
+      <c r="G96" s="49"/>
+      <c r="H96" s="42"/>
     </row>
     <row r="97" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B97" s="10" t="str">
@@ -2479,8 +2365,8 @@
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
       <c r="F97" s="13"/>
-      <c r="G97" s="54"/>
-      <c r="H97" s="47"/>
+      <c r="G97" s="49"/>
+      <c r="H97" s="42"/>
     </row>
     <row r="98" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B98" s="10" t="str">
@@ -2491,8 +2377,8 @@
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
       <c r="F98" s="13"/>
-      <c r="G98" s="54"/>
-      <c r="H98" s="47"/>
+      <c r="G98" s="49"/>
+      <c r="H98" s="42"/>
     </row>
     <row r="99" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B99" s="10" t="str">
@@ -2503,8 +2389,8 @@
       <c r="D99" s="12"/>
       <c r="E99" s="12"/>
       <c r="F99" s="13"/>
-      <c r="G99" s="54"/>
-      <c r="H99" s="47"/>
+      <c r="G99" s="49"/>
+      <c r="H99" s="42"/>
     </row>
     <row r="100" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B100" s="10" t="str">
@@ -2515,8 +2401,8 @@
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
       <c r="F100" s="13"/>
-      <c r="G100" s="54"/>
-      <c r="H100" s="47"/>
+      <c r="G100" s="49"/>
+      <c r="H100" s="42"/>
     </row>
     <row r="101" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B101" s="10" t="str">
@@ -2527,8 +2413,8 @@
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
       <c r="F101" s="13"/>
-      <c r="G101" s="54"/>
-      <c r="H101" s="47"/>
+      <c r="G101" s="49"/>
+      <c r="H101" s="42"/>
     </row>
     <row r="102" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B102" s="10" t="str">
@@ -2539,8 +2425,8 @@
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
       <c r="F102" s="13"/>
-      <c r="G102" s="54"/>
-      <c r="H102" s="47"/>
+      <c r="G102" s="49"/>
+      <c r="H102" s="42"/>
     </row>
     <row r="103" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B103" s="10" t="str">
@@ -2551,8 +2437,8 @@
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
       <c r="F103" s="13"/>
-      <c r="G103" s="54"/>
-      <c r="H103" s="47"/>
+      <c r="G103" s="49"/>
+      <c r="H103" s="42"/>
     </row>
     <row r="104" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B104" s="10" t="str">
@@ -2563,8 +2449,8 @@
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
       <c r="F104" s="13"/>
-      <c r="G104" s="54"/>
-      <c r="H104" s="47"/>
+      <c r="G104" s="49"/>
+      <c r="H104" s="42"/>
     </row>
     <row r="105" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B105" s="10" t="str">
@@ -2575,8 +2461,8 @@
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
       <c r="F105" s="13"/>
-      <c r="G105" s="54"/>
-      <c r="H105" s="47"/>
+      <c r="G105" s="49"/>
+      <c r="H105" s="42"/>
     </row>
     <row r="106" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B106" s="10" t="str">
@@ -2587,8 +2473,8 @@
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
       <c r="F106" s="13"/>
-      <c r="G106" s="54"/>
-      <c r="H106" s="47"/>
+      <c r="G106" s="49"/>
+      <c r="H106" s="42"/>
     </row>
     <row r="107" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B107" s="10" t="str">
@@ -2599,8 +2485,8 @@
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
       <c r="F107" s="13"/>
-      <c r="G107" s="54"/>
-      <c r="H107" s="47"/>
+      <c r="G107" s="49"/>
+      <c r="H107" s="42"/>
     </row>
     <row r="108" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B108" s="10" t="str">
@@ -2611,8 +2497,8 @@
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
       <c r="F108" s="13"/>
-      <c r="G108" s="54"/>
-      <c r="H108" s="47"/>
+      <c r="G108" s="49"/>
+      <c r="H108" s="42"/>
     </row>
     <row r="109" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B109" s="10" t="str">
@@ -2623,8 +2509,8 @@
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
       <c r="F109" s="13"/>
-      <c r="G109" s="54"/>
-      <c r="H109" s="47"/>
+      <c r="G109" s="49"/>
+      <c r="H109" s="42"/>
     </row>
     <row r="110" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B110" s="10" t="str">
@@ -2635,8 +2521,8 @@
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
       <c r="F110" s="13"/>
-      <c r="G110" s="54"/>
-      <c r="H110" s="47"/>
+      <c r="G110" s="49"/>
+      <c r="H110" s="42"/>
     </row>
     <row r="111" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B111" s="6" t="str">
@@ -2647,8 +2533,8 @@
       <c r="D111" s="15"/>
       <c r="E111" s="15"/>
       <c r="F111" s="16"/>
-      <c r="G111" s="55"/>
-      <c r="H111" s="48"/>
+      <c r="G111" s="50"/>
+      <c r="H111" s="43"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2658,14 +2544,6 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="D7:H7"/>
   </mergeCells>
-  <conditionalFormatting sqref="K7:K8">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="✓">
-      <formula>NOT(ISERROR(SEARCH("✓",K7)))</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(K7))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H111" xr:uid="{61BFA409-FA25-4839-9962-B559577D526B}">
       <formula1>-10</formula1>
@@ -2695,1486 +2573,1563 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="10" style="23" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="23" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="23" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="23" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="3.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="10" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="19" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
+      <c r="A1" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
+      <c r="A2" s="72"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="26"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="C5" s="27" t="s">
+      <c r="A5" s="20"/>
+      <c r="C5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="28" t="str">
+      <c r="D5" s="24" t="str">
         <f>IF(Заполнение!D7="","",Заполнение!D7)</f>
-        <v>sdf</v>
-      </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="26"/>
+        <v/>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="C6" s="27" t="s">
+      <c r="A6" s="20"/>
+      <c r="C6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="28" t="str">
+      <c r="D6" s="24" t="str">
         <f>IF(Заполнение!D8="","",Заполнение!D8)</f>
-        <v>sdf</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="26"/>
+        <v/>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="C7" s="27" t="s">
+      <c r="A7" s="22"/>
+      <c r="C7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="60" t="str">
         <f>IF(Заполнение!D9="","",Заполнение!D9)</f>
-        <v>45004</v>
-      </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="26"/>
+        <v/>
+      </c>
+      <c r="E7" s="60"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="70">
+      <c r="A8" s="22"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="59">
         <v>1</v>
       </c>
-      <c r="E8" s="70"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="26"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="26"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="75"/>
-      <c r="E10" s="31" t="s">
+      <c r="D10" s="66"/>
+      <c r="E10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="29" t="s">
-        <v>17</v>
+      <c r="G10" s="25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="33">
+      <c r="A11" s="29">
         <v>1</v>
       </c>
-      <c r="B11" s="34" t="str">
+      <c r="B11" s="30" t="str">
         <f>IF(Заполнение!C13="","",Заполнение!C13)</f>
-        <v>asdf</v>
-      </c>
-      <c r="C11" s="76" t="str">
+        <v/>
+      </c>
+      <c r="C11" s="67" t="str">
         <f>IF(Заполнение!D13="","",Заполнение!D13)</f>
-        <v>dsa</v>
-      </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="35" t="str">
+        <v/>
+      </c>
+      <c r="D11" s="68"/>
+      <c r="E11" s="31" t="str">
         <f>IF(Заполнение!E13="","",Заполнение!E13)</f>
-        <v>sd</v>
-      </c>
-      <c r="F11" s="35" t="str">
+        <v/>
+      </c>
+      <c r="F11" s="31" t="str">
         <f>IF(Заполнение!F13="","",Заполнение!F13)</f>
-        <v>Главный судья соревнований</v>
-      </c>
-      <c r="G11" s="33">
+        <v/>
+      </c>
+      <c r="G11" s="29" t="str">
         <f>IF(Заполнение!H13="","",Заполнение!H13)</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="str">
+      <c r="A12" s="29" t="str">
         <f t="shared" ref="A12" si="0">IF(B12&amp;C12&amp;E12="","",A11+1)</f>
         <v/>
       </c>
-      <c r="B12" s="34" t="str">
+      <c r="B12" s="30" t="str">
         <f>IF(Заполнение!C14="","",Заполнение!C14)</f>
         <v/>
       </c>
-      <c r="C12" s="66" t="str">
+      <c r="C12" s="63" t="str">
         <f>IF(Заполнение!D14="","",Заполнение!D14)</f>
         <v/>
       </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="35" t="str">
+      <c r="D12" s="64"/>
+      <c r="E12" s="31" t="str">
         <f>IF(Заполнение!E14="","",Заполнение!E14)</f>
         <v/>
       </c>
-      <c r="F12" s="36" t="str">
+      <c r="F12" s="32" t="str">
         <f>IF(Заполнение!F14="","",Заполнение!F14)</f>
         <v/>
       </c>
-      <c r="G12" s="33" t="str">
+      <c r="G12" s="29" t="str">
         <f>IF(Заполнение!H14="","",Заполнение!H14)</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="str">
+      <c r="A13" s="29" t="str">
         <f>IF(B13&amp;C13&amp;E13="","",A12+1)</f>
         <v/>
       </c>
-      <c r="B13" s="34" t="str">
+      <c r="B13" s="30" t="str">
         <f>IF(Заполнение!C15="","",Заполнение!C15)</f>
         <v/>
       </c>
-      <c r="C13" s="66" t="str">
+      <c r="C13" s="63" t="str">
         <f>IF(Заполнение!D15="","",Заполнение!D15)</f>
         <v/>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="35" t="str">
+      <c r="D13" s="64"/>
+      <c r="E13" s="31" t="str">
         <f>IF(Заполнение!E15="","",Заполнение!E15)</f>
         <v/>
       </c>
-      <c r="F13" s="36" t="str">
+      <c r="F13" s="32" t="str">
         <f>IF(Заполнение!F15="","",Заполнение!F15)</f>
         <v/>
       </c>
-      <c r="G13" s="33" t="str">
+      <c r="G13" s="29" t="str">
         <f>IF(Заполнение!H15="","",Заполнение!H15)</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="str">
+      <c r="A14" s="29" t="str">
         <f t="shared" ref="A14:A48" si="1">IF(B14&amp;C14&amp;E14="","",A13+1)</f>
         <v/>
       </c>
-      <c r="B14" s="34" t="str">
+      <c r="B14" s="30" t="str">
         <f>IF(Заполнение!C16="","",Заполнение!C16)</f>
         <v/>
       </c>
-      <c r="C14" s="66" t="str">
+      <c r="C14" s="63" t="str">
         <f>IF(Заполнение!D16="","",Заполнение!D16)</f>
         <v/>
       </c>
-      <c r="D14" s="67"/>
-      <c r="E14" s="35" t="str">
+      <c r="D14" s="64"/>
+      <c r="E14" s="31" t="str">
         <f>IF(Заполнение!E16="","",Заполнение!E16)</f>
         <v/>
       </c>
-      <c r="F14" s="36" t="str">
+      <c r="F14" s="32" t="str">
         <f>IF(Заполнение!F16="","",Заполнение!F16)</f>
         <v/>
       </c>
-      <c r="G14" s="33" t="str">
+      <c r="G14" s="29" t="str">
         <f>IF(Заполнение!H16="","",Заполнение!H16)</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B15" s="34" t="str">
+      <c r="A15" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B15" s="30" t="str">
         <f>IF(Заполнение!C17="","",Заполнение!C17)</f>
         <v/>
       </c>
-      <c r="C15" s="66" t="str">
+      <c r="C15" s="63" t="str">
         <f>IF(Заполнение!D17="","",Заполнение!D17)</f>
         <v/>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="35" t="str">
+      <c r="D15" s="64"/>
+      <c r="E15" s="31" t="str">
         <f>IF(Заполнение!E17="","",Заполнение!E17)</f>
         <v/>
       </c>
-      <c r="F15" s="36" t="str">
+      <c r="F15" s="32" t="str">
         <f>IF(Заполнение!F17="","",Заполнение!F17)</f>
         <v/>
       </c>
-      <c r="G15" s="33" t="str">
+      <c r="G15" s="29" t="str">
         <f>IF(Заполнение!H17="","",Заполнение!H17)</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B16" s="34" t="str">
+      <c r="A16" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B16" s="30" t="str">
         <f>IF(Заполнение!C18="","",Заполнение!C18)</f>
         <v/>
       </c>
-      <c r="C16" s="66" t="str">
+      <c r="C16" s="63" t="str">
         <f>IF(Заполнение!D18="","",Заполнение!D18)</f>
         <v/>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="35" t="str">
+      <c r="D16" s="64"/>
+      <c r="E16" s="31" t="str">
         <f>IF(Заполнение!E18="","",Заполнение!E18)</f>
         <v/>
       </c>
-      <c r="F16" s="36" t="str">
+      <c r="F16" s="32" t="str">
         <f>IF(Заполнение!F18="","",Заполнение!F18)</f>
         <v/>
       </c>
-      <c r="G16" s="33" t="str">
+      <c r="G16" s="29" t="str">
         <f>IF(Заполнение!H18="","",Заполнение!H18)</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B17" s="34" t="str">
+      <c r="A17" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B17" s="30" t="str">
         <f>IF(Заполнение!C19="","",Заполнение!C19)</f>
         <v/>
       </c>
-      <c r="C17" s="66" t="str">
+      <c r="C17" s="63" t="str">
         <f>IF(Заполнение!D19="","",Заполнение!D19)</f>
         <v/>
       </c>
-      <c r="D17" s="67"/>
-      <c r="E17" s="35" t="str">
+      <c r="D17" s="64"/>
+      <c r="E17" s="31" t="str">
         <f>IF(Заполнение!E19="","",Заполнение!E19)</f>
         <v/>
       </c>
-      <c r="F17" s="36" t="str">
+      <c r="F17" s="32" t="str">
         <f>IF(Заполнение!F19="","",Заполнение!F19)</f>
         <v/>
       </c>
-      <c r="G17" s="33" t="str">
+      <c r="G17" s="29" t="str">
         <f>IF(Заполнение!H19="","",Заполнение!H19)</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B18" s="34" t="str">
+      <c r="A18" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B18" s="30" t="str">
         <f>IF(Заполнение!C20="","",Заполнение!C20)</f>
         <v/>
       </c>
-      <c r="C18" s="66" t="str">
+      <c r="C18" s="63" t="str">
         <f>IF(Заполнение!D20="","",Заполнение!D20)</f>
         <v/>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="35" t="str">
+      <c r="D18" s="64"/>
+      <c r="E18" s="31" t="str">
         <f>IF(Заполнение!E20="","",Заполнение!E20)</f>
         <v/>
       </c>
-      <c r="F18" s="36" t="str">
+      <c r="F18" s="32" t="str">
         <f>IF(Заполнение!F20="","",Заполнение!F20)</f>
         <v/>
       </c>
-      <c r="G18" s="33" t="str">
+      <c r="G18" s="29" t="str">
         <f>IF(Заполнение!H20="","",Заполнение!H20)</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B19" s="34" t="str">
+      <c r="A19" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B19" s="30" t="str">
         <f>IF(Заполнение!C21="","",Заполнение!C21)</f>
         <v/>
       </c>
-      <c r="C19" s="66" t="str">
+      <c r="C19" s="63" t="str">
         <f>IF(Заполнение!D21="","",Заполнение!D21)</f>
         <v/>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="35" t="str">
+      <c r="D19" s="64"/>
+      <c r="E19" s="31" t="str">
         <f>IF(Заполнение!E21="","",Заполнение!E21)</f>
         <v/>
       </c>
-      <c r="F19" s="36" t="str">
+      <c r="F19" s="32" t="str">
         <f>IF(Заполнение!F21="","",Заполнение!F21)</f>
         <v/>
       </c>
-      <c r="G19" s="33" t="str">
+      <c r="G19" s="29" t="str">
         <f>IF(Заполнение!H21="","",Заполнение!H21)</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B20" s="34" t="str">
+      <c r="A20" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B20" s="30" t="str">
         <f>IF(Заполнение!C22="","",Заполнение!C22)</f>
         <v/>
       </c>
-      <c r="C20" s="66" t="str">
+      <c r="C20" s="63" t="str">
         <f>IF(Заполнение!D22="","",Заполнение!D22)</f>
         <v/>
       </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="35" t="str">
+      <c r="D20" s="64"/>
+      <c r="E20" s="31" t="str">
         <f>IF(Заполнение!E22="","",Заполнение!E22)</f>
         <v/>
       </c>
-      <c r="F20" s="36" t="str">
+      <c r="F20" s="32" t="str">
         <f>IF(Заполнение!F22="","",Заполнение!F22)</f>
         <v/>
       </c>
-      <c r="G20" s="33" t="str">
+      <c r="G20" s="29" t="str">
         <f>IF(Заполнение!H22="","",Заполнение!H22)</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B21" s="34" t="str">
+      <c r="A21" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B21" s="30" t="str">
         <f>IF(Заполнение!C23="","",Заполнение!C23)</f>
         <v/>
       </c>
-      <c r="C21" s="66" t="str">
+      <c r="C21" s="63" t="str">
         <f>IF(Заполнение!D23="","",Заполнение!D23)</f>
         <v/>
       </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="35" t="str">
+      <c r="D21" s="64"/>
+      <c r="E21" s="31" t="str">
         <f>IF(Заполнение!E23="","",Заполнение!E23)</f>
         <v/>
       </c>
-      <c r="F21" s="36" t="str">
+      <c r="F21" s="32" t="str">
         <f>IF(Заполнение!F23="","",Заполнение!F23)</f>
         <v/>
       </c>
-      <c r="G21" s="33" t="str">
+      <c r="G21" s="29" t="str">
         <f>IF(Заполнение!H23="","",Заполнение!H23)</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B22" s="34" t="str">
+      <c r="A22" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B22" s="30" t="str">
         <f>IF(Заполнение!C24="","",Заполнение!C24)</f>
         <v/>
       </c>
-      <c r="C22" s="66" t="str">
+      <c r="C22" s="63" t="str">
         <f>IF(Заполнение!D24="","",Заполнение!D24)</f>
         <v/>
       </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="35" t="str">
+      <c r="D22" s="64"/>
+      <c r="E22" s="31" t="str">
         <f>IF(Заполнение!E24="","",Заполнение!E24)</f>
         <v/>
       </c>
-      <c r="F22" s="36" t="str">
+      <c r="F22" s="32" t="str">
         <f>IF(Заполнение!F24="","",Заполнение!F24)</f>
         <v/>
       </c>
-      <c r="G22" s="33" t="str">
+      <c r="G22" s="29" t="str">
         <f>IF(Заполнение!H24="","",Заполнение!H24)</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B23" s="34" t="str">
+      <c r="A23" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B23" s="30" t="str">
         <f>IF(Заполнение!C25="","",Заполнение!C25)</f>
         <v/>
       </c>
-      <c r="C23" s="66" t="str">
+      <c r="C23" s="63" t="str">
         <f>IF(Заполнение!D25="","",Заполнение!D25)</f>
         <v/>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="35" t="str">
+      <c r="D23" s="64"/>
+      <c r="E23" s="31" t="str">
         <f>IF(Заполнение!E25="","",Заполнение!E25)</f>
         <v/>
       </c>
-      <c r="F23" s="36" t="str">
+      <c r="F23" s="32" t="str">
         <f>IF(Заполнение!F25="","",Заполнение!F25)</f>
         <v/>
       </c>
-      <c r="G23" s="33" t="str">
+      <c r="G23" s="29" t="str">
         <f>IF(Заполнение!H25="","",Заполнение!H25)</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B24" s="34" t="str">
+      <c r="A24" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B24" s="30" t="str">
         <f>IF(Заполнение!C26="","",Заполнение!C26)</f>
         <v/>
       </c>
-      <c r="C24" s="66" t="str">
+      <c r="C24" s="63" t="str">
         <f>IF(Заполнение!D26="","",Заполнение!D26)</f>
         <v/>
       </c>
-      <c r="D24" s="67"/>
-      <c r="E24" s="35" t="str">
+      <c r="D24" s="64"/>
+      <c r="E24" s="31" t="str">
         <f>IF(Заполнение!E26="","",Заполнение!E26)</f>
         <v/>
       </c>
-      <c r="F24" s="36" t="str">
+      <c r="F24" s="32" t="str">
         <f>IF(Заполнение!F26="","",Заполнение!F26)</f>
         <v/>
       </c>
-      <c r="G24" s="33" t="str">
+      <c r="G24" s="29" t="str">
         <f>IF(Заполнение!H26="","",Заполнение!H26)</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B25" s="34" t="str">
+      <c r="A25" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B25" s="30" t="str">
         <f>IF(Заполнение!C27="","",Заполнение!C27)</f>
         <v/>
       </c>
-      <c r="C25" s="66" t="str">
+      <c r="C25" s="63" t="str">
         <f>IF(Заполнение!D27="","",Заполнение!D27)</f>
         <v/>
       </c>
-      <c r="D25" s="67"/>
-      <c r="E25" s="35" t="str">
+      <c r="D25" s="64"/>
+      <c r="E25" s="31" t="str">
         <f>IF(Заполнение!E27="","",Заполнение!E27)</f>
         <v/>
       </c>
-      <c r="F25" s="36" t="str">
+      <c r="F25" s="32" t="str">
         <f>IF(Заполнение!F27="","",Заполнение!F27)</f>
         <v/>
       </c>
-      <c r="G25" s="33" t="str">
+      <c r="G25" s="29" t="str">
         <f>IF(Заполнение!H27="","",Заполнение!H27)</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B26" s="34" t="str">
+      <c r="A26" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B26" s="30" t="str">
         <f>IF(Заполнение!C28="","",Заполнение!C28)</f>
         <v/>
       </c>
-      <c r="C26" s="66" t="str">
+      <c r="C26" s="63" t="str">
         <f>IF(Заполнение!D28="","",Заполнение!D28)</f>
         <v/>
       </c>
-      <c r="D26" s="67"/>
-      <c r="E26" s="35" t="str">
+      <c r="D26" s="64"/>
+      <c r="E26" s="31" t="str">
         <f>IF(Заполнение!E28="","",Заполнение!E28)</f>
         <v/>
       </c>
-      <c r="F26" s="36" t="str">
+      <c r="F26" s="32" t="str">
         <f>IF(Заполнение!F28="","",Заполнение!F28)</f>
         <v/>
       </c>
-      <c r="G26" s="33" t="str">
+      <c r="G26" s="29" t="str">
         <f>IF(Заполнение!H28="","",Заполнение!H28)</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B27" s="34" t="str">
+      <c r="A27" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B27" s="30" t="str">
         <f>IF(Заполнение!C29="","",Заполнение!C29)</f>
         <v/>
       </c>
-      <c r="C27" s="66" t="str">
+      <c r="C27" s="63" t="str">
         <f>IF(Заполнение!D29="","",Заполнение!D29)</f>
         <v/>
       </c>
-      <c r="D27" s="67"/>
-      <c r="E27" s="35" t="str">
+      <c r="D27" s="64"/>
+      <c r="E27" s="31" t="str">
         <f>IF(Заполнение!E29="","",Заполнение!E29)</f>
         <v/>
       </c>
-      <c r="F27" s="36" t="str">
+      <c r="F27" s="32" t="str">
         <f>IF(Заполнение!F29="","",Заполнение!F29)</f>
         <v/>
       </c>
-      <c r="G27" s="33" t="str">
+      <c r="G27" s="29" t="str">
         <f>IF(Заполнение!H29="","",Заполнение!H29)</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B28" s="34" t="str">
+      <c r="A28" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B28" s="30" t="str">
         <f>IF(Заполнение!C30="","",Заполнение!C30)</f>
         <v/>
       </c>
-      <c r="C28" s="66" t="str">
+      <c r="C28" s="63" t="str">
         <f>IF(Заполнение!D30="","",Заполнение!D30)</f>
         <v/>
       </c>
-      <c r="D28" s="67"/>
-      <c r="E28" s="35" t="str">
+      <c r="D28" s="64"/>
+      <c r="E28" s="31" t="str">
         <f>IF(Заполнение!E30="","",Заполнение!E30)</f>
         <v/>
       </c>
-      <c r="F28" s="36" t="str">
+      <c r="F28" s="32" t="str">
         <f>IF(Заполнение!F30="","",Заполнение!F30)</f>
         <v/>
       </c>
-      <c r="G28" s="33" t="str">
+      <c r="G28" s="29" t="str">
         <f>IF(Заполнение!H30="","",Заполнение!H30)</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B29" s="34" t="str">
+      <c r="A29" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B29" s="30" t="str">
         <f>IF(Заполнение!C31="","",Заполнение!C31)</f>
         <v/>
       </c>
-      <c r="C29" s="66" t="str">
+      <c r="C29" s="63" t="str">
         <f>IF(Заполнение!D31="","",Заполнение!D31)</f>
         <v/>
       </c>
-      <c r="D29" s="67"/>
-      <c r="E29" s="35" t="str">
+      <c r="D29" s="64"/>
+      <c r="E29" s="31" t="str">
         <f>IF(Заполнение!E31="","",Заполнение!E31)</f>
         <v/>
       </c>
-      <c r="F29" s="36" t="str">
+      <c r="F29" s="32" t="str">
         <f>IF(Заполнение!F31="","",Заполнение!F31)</f>
         <v/>
       </c>
-      <c r="G29" s="33" t="str">
+      <c r="G29" s="29" t="str">
         <f>IF(Заполнение!H31="","",Заполнение!H31)</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B30" s="34" t="str">
+      <c r="A30" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B30" s="30" t="str">
         <f>IF(Заполнение!C32="","",Заполнение!C32)</f>
         <v/>
       </c>
-      <c r="C30" s="66" t="str">
+      <c r="C30" s="63" t="str">
         <f>IF(Заполнение!D32="","",Заполнение!D32)</f>
         <v/>
       </c>
-      <c r="D30" s="67"/>
-      <c r="E30" s="35" t="str">
+      <c r="D30" s="64"/>
+      <c r="E30" s="31" t="str">
         <f>IF(Заполнение!E32="","",Заполнение!E32)</f>
         <v/>
       </c>
-      <c r="F30" s="36" t="str">
+      <c r="F30" s="32" t="str">
         <f>IF(Заполнение!F32="","",Заполнение!F32)</f>
         <v/>
       </c>
-      <c r="G30" s="33" t="str">
+      <c r="G30" s="29" t="str">
         <f>IF(Заполнение!H32="","",Заполнение!H32)</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B31" s="34" t="str">
+      <c r="A31" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B31" s="30" t="str">
         <f>IF(Заполнение!C33="","",Заполнение!C33)</f>
         <v/>
       </c>
-      <c r="C31" s="66" t="str">
+      <c r="C31" s="63" t="str">
         <f>IF(Заполнение!D33="","",Заполнение!D33)</f>
         <v/>
       </c>
-      <c r="D31" s="67"/>
-      <c r="E31" s="35" t="str">
+      <c r="D31" s="64"/>
+      <c r="E31" s="31" t="str">
         <f>IF(Заполнение!E33="","",Заполнение!E33)</f>
         <v/>
       </c>
-      <c r="F31" s="36" t="str">
+      <c r="F31" s="32" t="str">
         <f>IF(Заполнение!F33="","",Заполнение!F33)</f>
         <v/>
       </c>
-      <c r="G31" s="33" t="str">
+      <c r="G31" s="29" t="str">
         <f>IF(Заполнение!H33="","",Заполнение!H33)</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B32" s="34" t="str">
+      <c r="A32" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B32" s="30" t="str">
         <f>IF(Заполнение!C34="","",Заполнение!C34)</f>
         <v/>
       </c>
-      <c r="C32" s="66" t="str">
+      <c r="C32" s="63" t="str">
         <f>IF(Заполнение!D34="","",Заполнение!D34)</f>
         <v/>
       </c>
-      <c r="D32" s="67"/>
-      <c r="E32" s="35" t="str">
+      <c r="D32" s="64"/>
+      <c r="E32" s="31" t="str">
         <f>IF(Заполнение!E34="","",Заполнение!E34)</f>
         <v/>
       </c>
-      <c r="F32" s="36" t="str">
+      <c r="F32" s="32" t="str">
         <f>IF(Заполнение!F34="","",Заполнение!F34)</f>
         <v/>
       </c>
-      <c r="G32" s="33" t="str">
+      <c r="G32" s="29" t="str">
         <f>IF(Заполнение!H34="","",Заполнение!H34)</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B33" s="34" t="str">
+      <c r="A33" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B33" s="30" t="str">
         <f>IF(Заполнение!C35="","",Заполнение!C35)</f>
         <v/>
       </c>
-      <c r="C33" s="66" t="str">
+      <c r="C33" s="63" t="str">
         <f>IF(Заполнение!D35="","",Заполнение!D35)</f>
         <v/>
       </c>
-      <c r="D33" s="67"/>
-      <c r="E33" s="35" t="str">
+      <c r="D33" s="64"/>
+      <c r="E33" s="31" t="str">
         <f>IF(Заполнение!E35="","",Заполнение!E35)</f>
         <v/>
       </c>
-      <c r="F33" s="36" t="str">
+      <c r="F33" s="32" t="str">
         <f>IF(Заполнение!F35="","",Заполнение!F35)</f>
         <v/>
       </c>
-      <c r="G33" s="33" t="str">
+      <c r="G33" s="29" t="str">
         <f>IF(Заполнение!H35="","",Заполнение!H35)</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B34" s="34" t="str">
+      <c r="A34" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B34" s="30" t="str">
         <f>IF(Заполнение!C36="","",Заполнение!C36)</f>
         <v/>
       </c>
-      <c r="C34" s="66" t="str">
+      <c r="C34" s="63" t="str">
         <f>IF(Заполнение!D36="","",Заполнение!D36)</f>
         <v/>
       </c>
-      <c r="D34" s="67"/>
-      <c r="E34" s="35" t="str">
+      <c r="D34" s="64"/>
+      <c r="E34" s="31" t="str">
         <f>IF(Заполнение!E36="","",Заполнение!E36)</f>
         <v/>
       </c>
-      <c r="F34" s="36" t="str">
+      <c r="F34" s="32" t="str">
         <f>IF(Заполнение!F36="","",Заполнение!F36)</f>
         <v/>
       </c>
-      <c r="G34" s="33" t="str">
+      <c r="G34" s="29" t="str">
         <f>IF(Заполнение!H36="","",Заполнение!H36)</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B35" s="34" t="str">
+      <c r="A35" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B35" s="30" t="str">
         <f>IF(Заполнение!C37="","",Заполнение!C37)</f>
         <v/>
       </c>
-      <c r="C35" s="66" t="str">
+      <c r="C35" s="63" t="str">
         <f>IF(Заполнение!D37="","",Заполнение!D37)</f>
         <v/>
       </c>
-      <c r="D35" s="67"/>
-      <c r="E35" s="35" t="str">
+      <c r="D35" s="64"/>
+      <c r="E35" s="31" t="str">
         <f>IF(Заполнение!E37="","",Заполнение!E37)</f>
         <v/>
       </c>
-      <c r="F35" s="36" t="str">
+      <c r="F35" s="32" t="str">
         <f>IF(Заполнение!F37="","",Заполнение!F37)</f>
         <v/>
       </c>
-      <c r="G35" s="33" t="str">
+      <c r="G35" s="29" t="str">
         <f>IF(Заполнение!H37="","",Заполнение!H37)</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B36" s="34" t="str">
+      <c r="A36" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B36" s="30" t="str">
         <f>IF(Заполнение!C38="","",Заполнение!C38)</f>
         <v/>
       </c>
-      <c r="C36" s="66" t="str">
+      <c r="C36" s="63" t="str">
         <f>IF(Заполнение!D38="","",Заполнение!D38)</f>
         <v/>
       </c>
-      <c r="D36" s="67"/>
-      <c r="E36" s="35" t="str">
+      <c r="D36" s="64"/>
+      <c r="E36" s="31" t="str">
         <f>IF(Заполнение!E38="","",Заполнение!E38)</f>
         <v/>
       </c>
-      <c r="F36" s="36" t="str">
+      <c r="F36" s="32" t="str">
         <f>IF(Заполнение!F38="","",Заполнение!F38)</f>
         <v/>
       </c>
-      <c r="G36" s="33" t="str">
+      <c r="G36" s="29" t="str">
         <f>IF(Заполнение!H38="","",Заполнение!H38)</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B37" s="34" t="str">
+      <c r="A37" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B37" s="30" t="str">
         <f>IF(Заполнение!C39="","",Заполнение!C39)</f>
         <v/>
       </c>
-      <c r="C37" s="66" t="str">
+      <c r="C37" s="63" t="str">
         <f>IF(Заполнение!D39="","",Заполнение!D39)</f>
         <v/>
       </c>
-      <c r="D37" s="67"/>
-      <c r="E37" s="35" t="str">
+      <c r="D37" s="64"/>
+      <c r="E37" s="31" t="str">
         <f>IF(Заполнение!E39="","",Заполнение!E39)</f>
         <v/>
       </c>
-      <c r="F37" s="36" t="str">
+      <c r="F37" s="32" t="str">
         <f>IF(Заполнение!F39="","",Заполнение!F39)</f>
         <v/>
       </c>
-      <c r="G37" s="33" t="str">
+      <c r="G37" s="29" t="str">
         <f>IF(Заполнение!H39="","",Заполнение!H39)</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B38" s="34" t="str">
+      <c r="A38" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B38" s="30" t="str">
         <f>IF(Заполнение!C40="","",Заполнение!C40)</f>
         <v/>
       </c>
-      <c r="C38" s="66" t="str">
+      <c r="C38" s="63" t="str">
         <f>IF(Заполнение!D40="","",Заполнение!D40)</f>
         <v/>
       </c>
-      <c r="D38" s="67"/>
-      <c r="E38" s="35" t="str">
+      <c r="D38" s="64"/>
+      <c r="E38" s="31" t="str">
         <f>IF(Заполнение!E40="","",Заполнение!E40)</f>
         <v/>
       </c>
-      <c r="F38" s="36" t="str">
+      <c r="F38" s="32" t="str">
         <f>IF(Заполнение!F40="","",Заполнение!F40)</f>
         <v/>
       </c>
-      <c r="G38" s="33" t="str">
+      <c r="G38" s="29" t="str">
         <f>IF(Заполнение!H40="","",Заполнение!H40)</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B39" s="34" t="str">
+      <c r="A39" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B39" s="30" t="str">
         <f>IF(Заполнение!C41="","",Заполнение!C41)</f>
         <v/>
       </c>
-      <c r="C39" s="66" t="str">
+      <c r="C39" s="63" t="str">
         <f>IF(Заполнение!D41="","",Заполнение!D41)</f>
         <v/>
       </c>
-      <c r="D39" s="67"/>
-      <c r="E39" s="35" t="str">
+      <c r="D39" s="64"/>
+      <c r="E39" s="31" t="str">
         <f>IF(Заполнение!E41="","",Заполнение!E41)</f>
         <v/>
       </c>
-      <c r="F39" s="36" t="str">
+      <c r="F39" s="32" t="str">
         <f>IF(Заполнение!F41="","",Заполнение!F41)</f>
         <v/>
       </c>
-      <c r="G39" s="33" t="str">
+      <c r="G39" s="29" t="str">
         <f>IF(Заполнение!H41="","",Заполнение!H41)</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B40" s="34" t="str">
+      <c r="A40" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B40" s="30" t="str">
         <f>IF(Заполнение!C42="","",Заполнение!C42)</f>
         <v/>
       </c>
-      <c r="C40" s="66" t="str">
+      <c r="C40" s="63" t="str">
         <f>IF(Заполнение!D42="","",Заполнение!D42)</f>
         <v/>
       </c>
-      <c r="D40" s="67"/>
-      <c r="E40" s="35" t="str">
+      <c r="D40" s="64"/>
+      <c r="E40" s="31" t="str">
         <f>IF(Заполнение!E42="","",Заполнение!E42)</f>
         <v/>
       </c>
-      <c r="F40" s="36" t="str">
+      <c r="F40" s="32" t="str">
         <f>IF(Заполнение!F42="","",Заполнение!F42)</f>
         <v/>
       </c>
-      <c r="G40" s="33" t="str">
+      <c r="G40" s="29" t="str">
         <f>IF(Заполнение!H42="","",Заполнение!H42)</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B41" s="34" t="str">
+      <c r="A41" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B41" s="30" t="str">
         <f>IF(Заполнение!C43="","",Заполнение!C43)</f>
         <v/>
       </c>
-      <c r="C41" s="66" t="str">
+      <c r="C41" s="63" t="str">
         <f>IF(Заполнение!D43="","",Заполнение!D43)</f>
         <v/>
       </c>
-      <c r="D41" s="67"/>
-      <c r="E41" s="35" t="str">
+      <c r="D41" s="64"/>
+      <c r="E41" s="31" t="str">
         <f>IF(Заполнение!E43="","",Заполнение!E43)</f>
         <v/>
       </c>
-      <c r="F41" s="36" t="str">
+      <c r="F41" s="32" t="str">
         <f>IF(Заполнение!F43="","",Заполнение!F43)</f>
         <v/>
       </c>
-      <c r="G41" s="33" t="str">
+      <c r="G41" s="29" t="str">
         <f>IF(Заполнение!H43="","",Заполнение!H43)</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B42" s="34" t="str">
+      <c r="A42" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B42" s="30" t="str">
         <f>IF(Заполнение!C44="","",Заполнение!C44)</f>
         <v/>
       </c>
-      <c r="C42" s="66" t="str">
+      <c r="C42" s="63" t="str">
         <f>IF(Заполнение!D44="","",Заполнение!D44)</f>
         <v/>
       </c>
-      <c r="D42" s="67"/>
-      <c r="E42" s="35" t="str">
+      <c r="D42" s="64"/>
+      <c r="E42" s="31" t="str">
         <f>IF(Заполнение!E44="","",Заполнение!E44)</f>
         <v/>
       </c>
-      <c r="F42" s="36" t="str">
+      <c r="F42" s="32" t="str">
         <f>IF(Заполнение!F44="","",Заполнение!F44)</f>
         <v/>
       </c>
-      <c r="G42" s="33" t="str">
+      <c r="G42" s="29" t="str">
         <f>IF(Заполнение!H44="","",Заполнение!H44)</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B43" s="34" t="str">
+      <c r="A43" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B43" s="30" t="str">
         <f>IF(Заполнение!C45="","",Заполнение!C45)</f>
         <v/>
       </c>
-      <c r="C43" s="66" t="str">
+      <c r="C43" s="63" t="str">
         <f>IF(Заполнение!D45="","",Заполнение!D45)</f>
         <v/>
       </c>
-      <c r="D43" s="67"/>
-      <c r="E43" s="35" t="str">
+      <c r="D43" s="64"/>
+      <c r="E43" s="31" t="str">
         <f>IF(Заполнение!E45="","",Заполнение!E45)</f>
         <v/>
       </c>
-      <c r="F43" s="36" t="str">
+      <c r="F43" s="32" t="str">
         <f>IF(Заполнение!F45="","",Заполнение!F45)</f>
         <v/>
       </c>
-      <c r="G43" s="33" t="str">
+      <c r="G43" s="29" t="str">
         <f>IF(Заполнение!H45="","",Заполнение!H45)</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B44" s="34" t="str">
+      <c r="A44" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B44" s="30" t="str">
         <f>IF(Заполнение!C46="","",Заполнение!C46)</f>
         <v/>
       </c>
-      <c r="C44" s="66" t="str">
+      <c r="C44" s="63" t="str">
         <f>IF(Заполнение!D46="","",Заполнение!D46)</f>
         <v/>
       </c>
-      <c r="D44" s="67"/>
-      <c r="E44" s="35" t="str">
+      <c r="D44" s="64"/>
+      <c r="E44" s="31" t="str">
         <f>IF(Заполнение!E46="","",Заполнение!E46)</f>
         <v/>
       </c>
-      <c r="F44" s="36" t="str">
+      <c r="F44" s="32" t="str">
         <f>IF(Заполнение!F46="","",Заполнение!F46)</f>
         <v/>
       </c>
-      <c r="G44" s="33" t="str">
+      <c r="G44" s="29" t="str">
         <f>IF(Заполнение!H46="","",Заполнение!H46)</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B45" s="34" t="str">
+      <c r="A45" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B45" s="30" t="str">
         <f>IF(Заполнение!C47="","",Заполнение!C47)</f>
         <v/>
       </c>
-      <c r="C45" s="66" t="str">
+      <c r="C45" s="63" t="str">
         <f>IF(Заполнение!D47="","",Заполнение!D47)</f>
         <v/>
       </c>
-      <c r="D45" s="67"/>
-      <c r="E45" s="35" t="str">
+      <c r="D45" s="64"/>
+      <c r="E45" s="31" t="str">
         <f>IF(Заполнение!E47="","",Заполнение!E47)</f>
         <v/>
       </c>
-      <c r="F45" s="36" t="str">
+      <c r="F45" s="32" t="str">
         <f>IF(Заполнение!F47="","",Заполнение!F47)</f>
         <v/>
       </c>
-      <c r="G45" s="33" t="str">
+      <c r="G45" s="29" t="str">
         <f>IF(Заполнение!H47="","",Заполнение!H47)</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B46" s="34" t="str">
+      <c r="A46" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B46" s="30" t="str">
         <f>IF(Заполнение!C48="","",Заполнение!C48)</f>
         <v/>
       </c>
-      <c r="C46" s="66" t="str">
+      <c r="C46" s="63" t="str">
         <f>IF(Заполнение!D48="","",Заполнение!D48)</f>
         <v/>
       </c>
-      <c r="D46" s="67"/>
-      <c r="E46" s="35" t="str">
+      <c r="D46" s="64"/>
+      <c r="E46" s="31" t="str">
         <f>IF(Заполнение!E48="","",Заполнение!E48)</f>
         <v/>
       </c>
-      <c r="F46" s="36" t="str">
+      <c r="F46" s="32" t="str">
         <f>IF(Заполнение!F48="","",Заполнение!F48)</f>
         <v/>
       </c>
-      <c r="G46" s="33" t="str">
+      <c r="G46" s="29" t="str">
         <f>IF(Заполнение!H48="","",Заполнение!H48)</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B47" s="34" t="str">
+      <c r="A47" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B47" s="30" t="str">
         <f>IF(Заполнение!C49="","",Заполнение!C49)</f>
         <v/>
       </c>
-      <c r="C47" s="66" t="str">
+      <c r="C47" s="63" t="str">
         <f>IF(Заполнение!D49="","",Заполнение!D49)</f>
         <v/>
       </c>
-      <c r="D47" s="67"/>
-      <c r="E47" s="35" t="str">
+      <c r="D47" s="64"/>
+      <c r="E47" s="31" t="str">
         <f>IF(Заполнение!E49="","",Заполнение!E49)</f>
         <v/>
       </c>
-      <c r="F47" s="36" t="str">
+      <c r="F47" s="32" t="str">
         <f>IF(Заполнение!F49="","",Заполнение!F49)</f>
         <v/>
       </c>
-      <c r="G47" s="33" t="str">
+      <c r="G47" s="29" t="str">
         <f>IF(Заполнение!H49="","",Заполнение!H49)</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="49" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B48" s="38" t="str">
+      <c r="A48" s="44" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B48" s="34" t="str">
         <f>IF(Заполнение!C50="","",Заполнение!C50)</f>
         <v/>
       </c>
-      <c r="C48" s="68" t="str">
+      <c r="C48" s="70" t="str">
         <f>IF(Заполнение!D50="","",Заполнение!D50)</f>
         <v/>
       </c>
-      <c r="D48" s="69"/>
-      <c r="E48" s="39" t="str">
+      <c r="D48" s="71"/>
+      <c r="E48" s="35" t="str">
         <f>IF(Заполнение!E50="","",Заполнение!E50)</f>
         <v/>
       </c>
-      <c r="F48" s="40" t="str">
+      <c r="F48" s="36" t="str">
         <f>IF(Заполнение!F50="","",Заполнение!F50)</f>
         <v/>
       </c>
-      <c r="G48" s="37" t="str">
+      <c r="G48" s="33" t="str">
         <f>IF(Заполнение!H50="","",Заполнение!H50)</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="G49" s="23"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="G49" s="19"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="72" t="s">
+      <c r="A51" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="61"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="62"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="61"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="72"/>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="G51" s="73"/>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="72"/>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="73" t="s">
-        <v>31</v>
-      </c>
-      <c r="G52" s="73"/>
+      <c r="G52" s="62"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="72" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="72"/>
-      <c r="C53" s="72"/>
-      <c r="D53" s="72"/>
-      <c r="E53" s="72"/>
-      <c r="F53" s="73" t="str">
+      <c r="A53" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="62" t="str">
         <f ca="1">"Дата: " &amp; TEXT(TODAY(),"ДД.ММ.ГГГГ")</f>
-        <v>Дата: 19.03.2023</v>
-      </c>
-      <c r="G53" s="73"/>
-      <c r="I53" s="46"/>
+        <v>Дата: 21.03.2023</v>
+      </c>
+      <c r="G53" s="62"/>
+      <c r="I53" s="41"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="64"/>
-      <c r="D54" s="64"/>
-      <c r="G54" s="23"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="69"/>
+      <c r="G54" s="19"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="64"/>
-      <c r="D55" s="64"/>
-      <c r="G55" s="23"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="G55" s="19"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="64"/>
-      <c r="D56" s="64"/>
-      <c r="G56" s="23"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
+      <c r="G56" s="19"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="64"/>
-      <c r="D57" s="64"/>
-      <c r="G57" s="23"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="69"/>
+      <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="64"/>
-      <c r="D58" s="64"/>
-      <c r="G58" s="23"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="69"/>
+      <c r="G58" s="19"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="64"/>
-      <c r="D62" s="64"/>
-      <c r="G62" s="23"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="69"/>
+      <c r="G62" s="19"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
-      <c r="G63" s="23"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="69"/>
+      <c r="G63" s="19"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C64" s="64"/>
-      <c r="D64" s="64"/>
-      <c r="G64" s="23"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="69"/>
+      <c r="G64" s="19"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="64"/>
-      <c r="D65" s="64"/>
-      <c r="G65" s="23"/>
+      <c r="C65" s="69"/>
+      <c r="D65" s="69"/>
+      <c r="G65" s="19"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
-      <c r="G66" s="23"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="69"/>
+      <c r="G66" s="19"/>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="64"/>
-      <c r="D67" s="64"/>
-      <c r="G67" s="23"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="69"/>
+      <c r="G67" s="19"/>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="64"/>
-      <c r="D68" s="64"/>
-      <c r="G68" s="23"/>
+      <c r="C68" s="69"/>
+      <c r="D68" s="69"/>
+      <c r="G68" s="19"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="64"/>
-      <c r="D69" s="64"/>
-      <c r="G69" s="23"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="69"/>
+      <c r="G69" s="19"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
-      <c r="G70" s="23"/>
+      <c r="C70" s="69"/>
+      <c r="D70" s="69"/>
+      <c r="G70" s="19"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="64"/>
-      <c r="D71" s="64"/>
-      <c r="G71" s="23"/>
+      <c r="C71" s="69"/>
+      <c r="D71" s="69"/>
+      <c r="G71" s="19"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
-      <c r="G72" s="23"/>
+      <c r="C72" s="69"/>
+      <c r="D72" s="69"/>
+      <c r="G72" s="19"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="64"/>
-      <c r="D73" s="64"/>
-      <c r="G73" s="23"/>
+      <c r="C73" s="69"/>
+      <c r="D73" s="69"/>
+      <c r="G73" s="19"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="64"/>
-      <c r="D74" s="64"/>
-      <c r="G74" s="23"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
+      <c r="G74" s="19"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="64"/>
-      <c r="D75" s="64"/>
-      <c r="G75" s="23"/>
+      <c r="C75" s="69"/>
+      <c r="D75" s="69"/>
+      <c r="G75" s="19"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="64"/>
-      <c r="D76" s="64"/>
-      <c r="G76" s="23"/>
+      <c r="C76" s="69"/>
+      <c r="D76" s="69"/>
+      <c r="G76" s="19"/>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="64"/>
-      <c r="D77" s="64"/>
-      <c r="G77" s="23"/>
+      <c r="C77" s="69"/>
+      <c r="D77" s="69"/>
+      <c r="G77" s="19"/>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="64"/>
-      <c r="D78" s="64"/>
-      <c r="G78" s="23"/>
+      <c r="C78" s="69"/>
+      <c r="D78" s="69"/>
+      <c r="G78" s="19"/>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="64"/>
-      <c r="D79" s="64"/>
-      <c r="G79" s="23"/>
+      <c r="C79" s="69"/>
+      <c r="D79" s="69"/>
+      <c r="G79" s="19"/>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="64"/>
-      <c r="D80" s="64"/>
-      <c r="G80" s="23"/>
+      <c r="C80" s="69"/>
+      <c r="D80" s="69"/>
+      <c r="G80" s="19"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="64"/>
-      <c r="D81" s="64"/>
-      <c r="G81" s="23"/>
+      <c r="C81" s="69"/>
+      <c r="D81" s="69"/>
+      <c r="G81" s="19"/>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="64"/>
-      <c r="D82" s="64"/>
-      <c r="G82" s="23"/>
+      <c r="C82" s="69"/>
+      <c r="D82" s="69"/>
+      <c r="G82" s="19"/>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="64"/>
-      <c r="D83" s="64"/>
-      <c r="G83" s="23"/>
+      <c r="C83" s="69"/>
+      <c r="D83" s="69"/>
+      <c r="G83" s="19"/>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="64"/>
-      <c r="D84" s="64"/>
-      <c r="G84" s="23"/>
+      <c r="C84" s="69"/>
+      <c r="D84" s="69"/>
+      <c r="G84" s="19"/>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="64"/>
-      <c r="D85" s="64"/>
-      <c r="G85" s="23"/>
+      <c r="C85" s="69"/>
+      <c r="D85" s="69"/>
+      <c r="G85" s="19"/>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="64"/>
-      <c r="D86" s="64"/>
-      <c r="G86" s="23"/>
+      <c r="C86" s="69"/>
+      <c r="D86" s="69"/>
+      <c r="G86" s="19"/>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="64"/>
-      <c r="D87" s="64"/>
-      <c r="G87" s="23"/>
+      <c r="C87" s="69"/>
+      <c r="D87" s="69"/>
+      <c r="G87" s="19"/>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="64"/>
-      <c r="D88" s="64"/>
-      <c r="G88" s="23"/>
+      <c r="C88" s="69"/>
+      <c r="D88" s="69"/>
+      <c r="G88" s="19"/>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="64"/>
-      <c r="D89" s="64"/>
-      <c r="G89" s="23"/>
+      <c r="C89" s="69"/>
+      <c r="D89" s="69"/>
+      <c r="G89" s="19"/>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="64"/>
-      <c r="D90" s="64"/>
-      <c r="G90" s="23"/>
+      <c r="C90" s="69"/>
+      <c r="D90" s="69"/>
+      <c r="G90" s="19"/>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="64"/>
-      <c r="D91" s="64"/>
-      <c r="G91" s="23"/>
+      <c r="C91" s="69"/>
+      <c r="D91" s="69"/>
+      <c r="G91" s="19"/>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="64"/>
-      <c r="D92" s="64"/>
-      <c r="G92" s="23"/>
+      <c r="C92" s="69"/>
+      <c r="D92" s="69"/>
+      <c r="G92" s="19"/>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="64"/>
-      <c r="D93" s="64"/>
-      <c r="G93" s="23"/>
+      <c r="C93" s="69"/>
+      <c r="D93" s="69"/>
+      <c r="G93" s="19"/>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="64"/>
-      <c r="D94" s="64"/>
-      <c r="G94" s="23"/>
+      <c r="C94" s="69"/>
+      <c r="D94" s="69"/>
+      <c r="G94" s="19"/>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C95" s="64"/>
-      <c r="D95" s="64"/>
-      <c r="G95" s="23"/>
+      <c r="C95" s="69"/>
+      <c r="D95" s="69"/>
+      <c r="G95" s="19"/>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C96" s="64"/>
-      <c r="D96" s="64"/>
-      <c r="G96" s="23"/>
+      <c r="C96" s="69"/>
+      <c r="D96" s="69"/>
+      <c r="G96" s="19"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C97" s="64"/>
-      <c r="D97" s="64"/>
-      <c r="G97" s="23"/>
+      <c r="C97" s="69"/>
+      <c r="D97" s="69"/>
+      <c r="G97" s="19"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C98" s="64"/>
-      <c r="D98" s="64"/>
-      <c r="G98" s="23"/>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
+      <c r="G98" s="19"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C99" s="64"/>
-      <c r="D99" s="64"/>
-      <c r="G99" s="23"/>
+      <c r="C99" s="69"/>
+      <c r="D99" s="69"/>
+      <c r="G99" s="19"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C100" s="64"/>
-      <c r="D100" s="64"/>
-      <c r="G100" s="23"/>
+      <c r="C100" s="69"/>
+      <c r="D100" s="69"/>
+      <c r="G100" s="19"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C101" s="64"/>
-      <c r="D101" s="64"/>
-      <c r="G101" s="23"/>
+      <c r="C101" s="69"/>
+      <c r="D101" s="69"/>
+      <c r="G101" s="19"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C102" s="64"/>
-      <c r="D102" s="64"/>
-      <c r="G102" s="23"/>
+      <c r="C102" s="69"/>
+      <c r="D102" s="69"/>
+      <c r="G102" s="19"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C103" s="64"/>
-      <c r="D103" s="64"/>
-      <c r="G103" s="23"/>
+      <c r="C103" s="69"/>
+      <c r="D103" s="69"/>
+      <c r="G103" s="19"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C104" s="64"/>
-      <c r="D104" s="64"/>
-      <c r="G104" s="23"/>
+      <c r="C104" s="69"/>
+      <c r="D104" s="69"/>
+      <c r="G104" s="19"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C105" s="64"/>
-      <c r="D105" s="64"/>
-      <c r="G105" s="23"/>
+      <c r="C105" s="69"/>
+      <c r="D105" s="69"/>
+      <c r="G105" s="19"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C106" s="64"/>
-      <c r="D106" s="64"/>
-      <c r="G106" s="23"/>
+      <c r="C106" s="69"/>
+      <c r="D106" s="69"/>
+      <c r="G106" s="19"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C107" s="64"/>
-      <c r="D107" s="64"/>
-      <c r="G107" s="23"/>
+      <c r="C107" s="69"/>
+      <c r="D107" s="69"/>
+      <c r="G107" s="19"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C108" s="64"/>
-      <c r="D108" s="64"/>
-      <c r="G108" s="23"/>
+      <c r="C108" s="69"/>
+      <c r="D108" s="69"/>
+      <c r="G108" s="19"/>
     </row>
     <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="41"/>
-      <c r="B110" s="42"/>
-      <c r="C110" s="42"/>
-      <c r="D110" s="43"/>
-      <c r="E110" s="42"/>
-      <c r="F110" s="42"/>
-      <c r="G110" s="41"/>
-      <c r="H110" s="42"/>
-      <c r="I110" s="41"/>
+      <c r="A110" s="37"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="38"/>
+      <c r="D110" s="39"/>
+      <c r="E110" s="38"/>
+      <c r="F110" s="38"/>
+      <c r="G110" s="37"/>
+      <c r="H110" s="38"/>
+      <c r="I110" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="101">
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="A1:G3"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="A53:E53"/>
@@ -4199,83 +4154,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="A1:G3"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C82:D82"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0" header="0" footer="0"/>

</xml_diff>